<commit_message>
updates to jcp dmd excels
</commit_message>
<xml_diff>
--- a/jcp-dmd/Base Data Model.xlsx
+++ b/jcp-dmd/Base Data Model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="33520" windowHeight="20540" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="33520" windowHeight="20540" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="HELP" sheetId="19" r:id="rId1"/>
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4221" uniqueCount="1169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4223" uniqueCount="1169">
   <si>
     <t>ACTION</t>
   </si>
@@ -4709,11 +4709,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE356"/>
+  <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
+  <dimension ref="A1:AE1465"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A34" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1472" sqref="C1472"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4844,7 +4845,7 @@
         <v>899</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>1027</v>
       </c>
@@ -4865,7 +4866,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1138</v>
       </c>
@@ -4892,7 +4893,7 @@
         <v>1141</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="27" t="s">
         <v>502</v>
       </c>
@@ -4913,7 +4914,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
         <v>503</v>
       </c>
@@ -4934,7 +4935,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
         <v>504</v>
       </c>
@@ -4955,7 +4956,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
         <v>505</v>
       </c>
@@ -4976,7 +4977,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="27" t="s">
         <v>102</v>
       </c>
@@ -5003,7 +5004,7 @@
         <v>909</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="28" t="s">
         <v>506</v>
       </c>
@@ -5033,7 +5034,7 @@
         <v>910</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B10" s="27" t="s">
         <v>103</v>
       </c>
@@ -5060,7 +5061,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B11" s="28" t="s">
         <v>104</v>
       </c>
@@ -5087,7 +5088,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B12" s="28" t="s">
         <v>105</v>
       </c>
@@ -5117,7 +5118,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B13" s="28" t="s">
         <v>507</v>
       </c>
@@ -5150,7 +5151,7 @@
         <v>905</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B14" s="28" t="s">
         <v>106</v>
       </c>
@@ -5180,7 +5181,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B15" s="28" t="s">
         <v>508</v>
       </c>
@@ -5210,7 +5211,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B16" s="28" t="s">
         <v>509</v>
       </c>
@@ -5243,7 +5244,7 @@
         <v>970</v>
       </c>
     </row>
-    <row r="17" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B17" s="28" t="s">
         <v>510</v>
       </c>
@@ -5276,7 +5277,7 @@
         <v>971</v>
       </c>
     </row>
-    <row r="18" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B18" s="28" t="s">
         <v>511</v>
       </c>
@@ -5309,7 +5310,7 @@
         <v>972</v>
       </c>
     </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B19" s="28" t="s">
         <v>512</v>
       </c>
@@ -5342,7 +5343,7 @@
         <v>1089</v>
       </c>
     </row>
-    <row r="20" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B20" s="28" t="s">
         <v>109</v>
       </c>
@@ -5375,7 +5376,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="21" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B21" s="29" t="s">
         <v>513</v>
       </c>
@@ -5405,7 +5406,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="22" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B22" s="27" t="s">
         <v>110</v>
       </c>
@@ -5432,7 +5433,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="23" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B23" s="28" t="s">
         <v>514</v>
       </c>
@@ -5465,7 +5466,7 @@
         <v>906</v>
       </c>
     </row>
-    <row r="24" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B24" s="28" t="s">
         <v>515</v>
       </c>
@@ -5486,7 +5487,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="25" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B25" s="28" t="s">
         <v>111</v>
       </c>
@@ -5519,7 +5520,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="26" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B26" s="27" t="s">
         <v>516</v>
       </c>
@@ -5555,7 +5556,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="27" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B27" s="27" t="s">
         <v>517</v>
       </c>
@@ -5591,7 +5592,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="28" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B28" s="27" t="s">
         <v>518</v>
       </c>
@@ -5627,7 +5628,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="29" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B29" s="27" t="s">
         <v>519</v>
       </c>
@@ -5663,7 +5664,7 @@
         <v>938</v>
       </c>
     </row>
-    <row r="30" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B30" s="27" t="s">
         <v>520</v>
       </c>
@@ -5696,7 +5697,7 @@
         <v>933</v>
       </c>
     </row>
-    <row r="31" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B31" s="27" t="s">
         <v>521</v>
       </c>
@@ -5729,7 +5730,7 @@
         <v>937</v>
       </c>
     </row>
-    <row r="32" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B32" s="27" t="s">
         <v>522</v>
       </c>
@@ -5762,7 +5763,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="33" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B33" s="27" t="s">
         <v>523</v>
       </c>
@@ -5822,7 +5823,7 @@
         <v>923</v>
       </c>
     </row>
-    <row r="35" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>525</v>
       </c>
@@ -5855,7 +5856,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="36" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>526</v>
       </c>
@@ -5882,7 +5883,7 @@
         <v>977</v>
       </c>
     </row>
-    <row r="37" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>527</v>
       </c>
@@ -5909,7 +5910,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="38" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>528</v>
       </c>
@@ -5936,7 +5937,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="39" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>529</v>
       </c>
@@ -5963,7 +5964,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="40" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>530</v>
       </c>
@@ -5990,7 +5991,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="41" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>531</v>
       </c>
@@ -6017,7 +6018,7 @@
         <v>927</v>
       </c>
     </row>
-    <row r="42" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>112</v>
       </c>
@@ -6053,7 +6054,7 @@
         <v>928</v>
       </c>
     </row>
-    <row r="43" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>532</v>
       </c>
@@ -6089,7 +6090,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="44" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>533</v>
       </c>
@@ -6125,7 +6126,7 @@
         <v>975</v>
       </c>
     </row>
-    <row r="45" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>32</v>
       </c>
@@ -6161,7 +6162,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="46" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>113</v>
       </c>
@@ -6191,7 +6192,7 @@
         <v>1003</v>
       </c>
     </row>
-    <row r="47" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>114</v>
       </c>
@@ -6221,7 +6222,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="48" spans="2:30" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:30" hidden="1" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>115</v>
       </c>
@@ -6251,7 +6252,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="49" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
         <v>534</v>
       </c>
@@ -6281,7 +6282,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="50" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>535</v>
       </c>
@@ -6311,7 +6312,7 @@
         <v>1006</v>
       </c>
     </row>
-    <row r="51" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>536</v>
       </c>
@@ -6344,7 +6345,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="52" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>537</v>
       </c>
@@ -6377,7 +6378,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="53" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>538</v>
       </c>
@@ -6410,7 +6411,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="54" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>539</v>
       </c>
@@ -6437,7 +6438,7 @@
         <v>930</v>
       </c>
     </row>
-    <row r="55" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B55" s="29" t="s">
         <v>540</v>
       </c>
@@ -6489,7 +6490,7 @@
       </c>
       <c r="AE55" s="29"/>
     </row>
-    <row r="56" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>541</v>
       </c>
@@ -6525,7 +6526,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="57" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>542</v>
       </c>
@@ -6558,7 +6559,7 @@
         <v>959</v>
       </c>
     </row>
-    <row r="58" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>543</v>
       </c>
@@ -6591,7 +6592,7 @@
         <v>960</v>
       </c>
     </row>
-    <row r="59" spans="2:31" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:31" hidden="1" x14ac:dyDescent="0.25">
       <c r="B59" t="s">
         <v>544</v>
       </c>
@@ -6624,7 +6625,7 @@
         <v>961</v>
       </c>
     </row>
-    <row r="60" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="60" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B60" t="s">
         <v>545</v>
       </c>
@@ -6657,7 +6658,7 @@
         <v>962</v>
       </c>
     </row>
-    <row r="61" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="61" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B61" t="s">
         <v>546</v>
       </c>
@@ -6690,7 +6691,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="62" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="62" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B62" t="s">
         <v>547</v>
       </c>
@@ -6720,7 +6721,7 @@
         <v>1015</v>
       </c>
     </row>
-    <row r="63" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="63" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B63" t="s">
         <v>39</v>
       </c>
@@ -6747,7 +6748,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="64" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="64" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
         <v>548</v>
       </c>
@@ -6777,7 +6778,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="65" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="65" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B65" t="s">
         <v>549</v>
       </c>
@@ -6807,7 +6808,7 @@
         <v>1018</v>
       </c>
     </row>
-    <row r="66" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="66" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B66" t="s">
         <v>550</v>
       </c>
@@ -6837,7 +6838,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="67" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="67" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
         <v>551</v>
       </c>
@@ -6870,7 +6871,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="68" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="68" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B68" t="s">
         <v>552</v>
       </c>
@@ -6897,7 +6898,7 @@
         <v>1021</v>
       </c>
     </row>
-    <row r="69" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="69" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B69" t="s">
         <v>116</v>
       </c>
@@ -6924,7 +6925,7 @@
         <v>1022</v>
       </c>
     </row>
-    <row r="70" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="70" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B70" t="s">
         <v>553</v>
       </c>
@@ -6951,7 +6952,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="71" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="71" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B71" t="s">
         <v>554</v>
       </c>
@@ -6978,7 +6979,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="72" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="72" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B72" t="s">
         <v>555</v>
       </c>
@@ -6999,7 +7000,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="73" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="73" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B73" t="s">
         <v>556</v>
       </c>
@@ -7032,7 +7033,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="74" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="74" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B74" t="s">
         <v>557</v>
       </c>
@@ -7065,7 +7066,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="75" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="75" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B75" t="s">
         <v>558</v>
       </c>
@@ -7092,7 +7093,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="76" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="76" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B76" t="s">
         <v>117</v>
       </c>
@@ -7122,7 +7123,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="77" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="77" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B77" t="s">
         <v>559</v>
       </c>
@@ -7149,7 +7150,7 @@
         <v>973</v>
       </c>
     </row>
-    <row r="78" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="78" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B78" t="s">
         <v>560</v>
       </c>
@@ -7176,7 +7177,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="79" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="79" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B79" t="s">
         <v>561</v>
       </c>
@@ -7209,7 +7210,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="80" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="80" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B80" t="s">
         <v>562</v>
       </c>
@@ -7242,7 +7243,7 @@
         <v>957</v>
       </c>
     </row>
-    <row r="81" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="81" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B81" t="s">
         <v>563</v>
       </c>
@@ -7275,7 +7276,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="82" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="82" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B82" t="s">
         <v>564</v>
       </c>
@@ -7302,7 +7303,7 @@
         <v>974</v>
       </c>
     </row>
-    <row r="83" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="83" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B83" t="s">
         <v>565</v>
       </c>
@@ -7329,7 +7330,7 @@
         <v>976</v>
       </c>
     </row>
-    <row r="84" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="84" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B84" t="s">
         <v>566</v>
       </c>
@@ -7362,7 +7363,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="85" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="85" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B85" t="s">
         <v>118</v>
       </c>
@@ -7395,7 +7396,7 @@
         <v>922</v>
       </c>
     </row>
-    <row r="86" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="86" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B86" t="s">
         <v>567</v>
       </c>
@@ -7422,7 +7423,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="87" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="87" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B87" t="s">
         <v>568</v>
       </c>
@@ -7449,7 +7450,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="88" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="88" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B88" t="s">
         <v>569</v>
       </c>
@@ -7482,7 +7483,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="89" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="89" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B89" t="s">
         <v>570</v>
       </c>
@@ -7515,7 +7516,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="90" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="90" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B90" t="s">
         <v>571</v>
       </c>
@@ -7548,7 +7549,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="91" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="91" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B91" t="s">
         <v>572</v>
       </c>
@@ -7575,7 +7576,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="92" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="92" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B92" t="s">
         <v>573</v>
       </c>
@@ -7602,7 +7603,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="93" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="93" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B93" t="s">
         <v>574</v>
       </c>
@@ -7635,7 +7636,7 @@
         <v>931</v>
       </c>
     </row>
-    <row r="94" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="94" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B94" t="s">
         <v>575</v>
       </c>
@@ -7668,7 +7669,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="95" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="95" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B95" t="s">
         <v>576</v>
       </c>
@@ -7701,7 +7702,7 @@
         <v>956</v>
       </c>
     </row>
-    <row r="96" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="96" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B96" t="s">
         <v>577</v>
       </c>
@@ -7731,7 +7732,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="97" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="97" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B97" t="s">
         <v>578</v>
       </c>
@@ -7764,7 +7765,7 @@
         <v>958</v>
       </c>
     </row>
-    <row r="98" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="98" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B98" t="s">
         <v>579</v>
       </c>
@@ -7797,7 +7798,7 @@
         <v>946</v>
       </c>
     </row>
-    <row r="99" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="99" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B99" t="s">
         <v>580</v>
       </c>
@@ -7830,7 +7831,7 @@
         <v>1026</v>
       </c>
     </row>
-    <row r="100" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="100" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B100" t="s">
         <v>581</v>
       </c>
@@ -7857,7 +7858,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="101" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="101" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B101" t="s">
         <v>582</v>
       </c>
@@ -7884,7 +7885,7 @@
         <v>947</v>
       </c>
     </row>
-    <row r="102" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="102" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B102" t="s">
         <v>583</v>
       </c>
@@ -7905,7 +7906,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="103" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="103" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B103" t="s">
         <v>584</v>
       </c>
@@ -7938,7 +7939,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="104" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="104" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B104" t="s">
         <v>585</v>
       </c>
@@ -7971,7 +7972,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="105" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="105" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B105" t="s">
         <v>586</v>
       </c>
@@ -8004,7 +8005,7 @@
         <v>1012</v>
       </c>
     </row>
-    <row r="106" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="106" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B106" t="s">
         <v>587</v>
       </c>
@@ -8037,7 +8038,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="107" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="107" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B107" t="s">
         <v>588</v>
       </c>
@@ -8070,7 +8071,7 @@
         <v>950</v>
       </c>
     </row>
-    <row r="108" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="108" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B108" t="s">
         <v>702</v>
       </c>
@@ -8103,7 +8104,7 @@
         <v>953</v>
       </c>
     </row>
-    <row r="109" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="109" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B109" t="s">
         <v>589</v>
       </c>
@@ -8130,7 +8131,7 @@
         <v>952</v>
       </c>
     </row>
-    <row r="110" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="110" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B110" t="s">
         <v>119</v>
       </c>
@@ -8163,7 +8164,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="111" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="111" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B111" t="s">
         <v>590</v>
       </c>
@@ -8190,7 +8191,7 @@
         <v>1023</v>
       </c>
     </row>
-    <row r="112" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="112" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B112" t="s">
         <v>591</v>
       </c>
@@ -8223,7 +8224,7 @@
         <v>1024</v>
       </c>
     </row>
-    <row r="113" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="113" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B113" t="s">
         <v>592</v>
       </c>
@@ -8250,7 +8251,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="114" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="114" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B114" t="s">
         <v>593</v>
       </c>
@@ -8277,7 +8278,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="115" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="115" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B115" t="s">
         <v>120</v>
       </c>
@@ -8310,7 +8311,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="116" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="116" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B116" t="s">
         <v>594</v>
       </c>
@@ -8346,7 +8347,7 @@
         <v>995</v>
       </c>
     </row>
-    <row r="117" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="117" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B117" t="s">
         <v>595</v>
       </c>
@@ -8373,7 +8374,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="118" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="118" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B118" t="s">
         <v>596</v>
       </c>
@@ -8406,7 +8407,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="119" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="119" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B119" t="s">
         <v>597</v>
       </c>
@@ -8439,7 +8440,7 @@
         <v>920</v>
       </c>
     </row>
-    <row r="120" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="120" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B120" t="s">
         <v>598</v>
       </c>
@@ -8472,7 +8473,7 @@
         <v>925</v>
       </c>
     </row>
-    <row r="121" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="121" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B121" t="s">
         <v>599</v>
       </c>
@@ -8505,7 +8506,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="122" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="122" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B122" t="s">
         <v>600</v>
       </c>
@@ -8538,7 +8539,7 @@
         <v>921</v>
       </c>
     </row>
-    <row r="123" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="123" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B123" t="s">
         <v>601</v>
       </c>
@@ -8571,7 +8572,7 @@
         <v>943</v>
       </c>
     </row>
-    <row r="124" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="124" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B124" t="s">
         <v>602</v>
       </c>
@@ -8598,7 +8599,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="125" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="125" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B125" t="s">
         <v>603</v>
       </c>
@@ -8631,7 +8632,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="126" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B126" t="s">
         <v>604</v>
       </c>
@@ -8658,7 +8659,7 @@
         <v>1009</v>
       </c>
     </row>
-    <row r="127" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="127" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B127" t="s">
         <v>605</v>
       </c>
@@ -8685,7 +8686,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="128" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="128" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B128" t="s">
         <v>606</v>
       </c>
@@ -8718,7 +8719,7 @@
         <v>949</v>
       </c>
     </row>
-    <row r="129" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B129" t="s">
         <v>607</v>
       </c>
@@ -8742,7 +8743,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="130" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="130" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B130" t="s">
         <v>608</v>
       </c>
@@ -8766,7 +8767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="131" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="131" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B131" t="s">
         <v>609</v>
       </c>
@@ -8790,7 +8791,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="132" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="132" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B132" t="s">
         <v>610</v>
       </c>
@@ -8814,7 +8815,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="133" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="133" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B133" t="s">
         <v>611</v>
       </c>
@@ -8838,7 +8839,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="134" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B134" t="s">
         <v>612</v>
       </c>
@@ -8859,7 +8860,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="135" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="135" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B135" t="s">
         <v>121</v>
       </c>
@@ -8880,7 +8881,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="136" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="136" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B136" t="s">
         <v>122</v>
       </c>
@@ -8901,7 +8902,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="137" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="137" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B137" t="s">
         <v>123</v>
       </c>
@@ -8922,7 +8923,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="138" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="138" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B138" t="s">
         <v>124</v>
       </c>
@@ -8943,7 +8944,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="139" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="139" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B139" t="s">
         <v>125</v>
       </c>
@@ -8964,7 +8965,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="140" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="140" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B140" t="s">
         <v>613</v>
       </c>
@@ -8985,7 +8986,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="141" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="141" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B141" t="s">
         <v>614</v>
       </c>
@@ -9015,7 +9016,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="142" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="142" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B142" t="s">
         <v>615</v>
       </c>
@@ -9036,7 +9037,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="143" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="143" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B143" t="s">
         <v>616</v>
       </c>
@@ -9057,7 +9058,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="144" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="144" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B144" t="s">
         <v>617</v>
       </c>
@@ -9087,7 +9088,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="145" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="145" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B145" t="s">
         <v>126</v>
       </c>
@@ -9117,7 +9118,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="146" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="146" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B146" t="s">
         <v>618</v>
       </c>
@@ -9156,7 +9157,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="147" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="147" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B147" t="s">
         <v>619</v>
       </c>
@@ -9186,7 +9187,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="148" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="148" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B148" t="s">
         <v>804</v>
       </c>
@@ -9216,7 +9217,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="149" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="149" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B149" s="27" t="s">
         <v>620</v>
       </c>
@@ -9236,7 +9237,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="150" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="150" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B150" s="27" t="s">
         <v>621</v>
       </c>
@@ -9256,7 +9257,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="151" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="151" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B151" s="27" t="s">
         <v>622</v>
       </c>
@@ -9276,7 +9277,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="152" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="152" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B152" s="27" t="s">
         <v>623</v>
       </c>
@@ -9296,7 +9297,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="153" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="153" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B153" s="27" t="s">
         <v>624</v>
       </c>
@@ -9316,7 +9317,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="154" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="154" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B154" s="27" t="s">
         <v>625</v>
       </c>
@@ -9336,7 +9337,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="155" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="155" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B155" s="27" t="s">
         <v>626</v>
       </c>
@@ -9356,7 +9357,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="156" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="156" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B156" s="27" t="s">
         <v>627</v>
       </c>
@@ -9376,7 +9377,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="157" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="157" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B157" s="27" t="s">
         <v>628</v>
       </c>
@@ -9396,7 +9397,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="158" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="158" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B158" s="27" t="s">
         <v>629</v>
       </c>
@@ -9416,7 +9417,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="159" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="159" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B159" s="27" t="s">
         <v>630</v>
       </c>
@@ -9436,7 +9437,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="160" spans="2:29" x14ac:dyDescent="0.2">
+    <row r="160" spans="2:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="B160" s="27" t="s">
         <v>631</v>
       </c>
@@ -9456,7 +9457,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="161" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="161" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B161" s="27" t="s">
         <v>632</v>
       </c>
@@ -9476,7 +9477,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="162" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="162" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B162" s="27" t="s">
         <v>633</v>
       </c>
@@ -9496,7 +9497,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="163" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="163" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B163" s="27" t="s">
         <v>634</v>
       </c>
@@ -9516,7 +9517,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="164" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="164" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B164" s="28" t="s">
         <v>635</v>
       </c>
@@ -9536,7 +9537,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="165" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="165" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B165" s="27" t="s">
         <v>636</v>
       </c>
@@ -9556,7 +9557,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="166" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="166" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B166" s="27" t="s">
         <v>637</v>
       </c>
@@ -9576,7 +9577,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="167" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="167" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B167" s="27" t="s">
         <v>638</v>
       </c>
@@ -9596,7 +9597,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="168" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="168" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B168" s="27" t="s">
         <v>639</v>
       </c>
@@ -9613,7 +9614,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="169" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="169" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B169" s="27" t="s">
         <v>640</v>
       </c>
@@ -9633,7 +9634,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="170" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="170" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B170" s="27" t="s">
         <v>641</v>
       </c>
@@ -9653,7 +9654,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="171" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="171" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B171" s="27" t="s">
         <v>642</v>
       </c>
@@ -9673,7 +9674,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="172" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="172" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B172" s="27" t="s">
         <v>643</v>
       </c>
@@ -9693,7 +9694,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="173" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="173" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B173" s="27" t="s">
         <v>644</v>
       </c>
@@ -9713,7 +9714,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="174" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="174" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B174" s="27" t="s">
         <v>645</v>
       </c>
@@ -9733,7 +9734,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="175" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="175" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B175" s="27" t="s">
         <v>646</v>
       </c>
@@ -9759,7 +9760,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="176" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="176" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B176" s="27" t="s">
         <v>647</v>
       </c>
@@ -9779,7 +9780,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="177" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="177" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B177" s="27" t="s">
         <v>648</v>
       </c>
@@ -9799,7 +9800,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="178" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="178" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B178" s="27" t="s">
         <v>649</v>
       </c>
@@ -9819,7 +9820,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="179" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="179" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B179" s="27" t="s">
         <v>650</v>
       </c>
@@ -9845,7 +9846,7 @@
         <v>969</v>
       </c>
     </row>
-    <row r="180" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="180" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B180" s="27" t="s">
         <v>651</v>
       </c>
@@ -9865,7 +9866,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="181" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="181" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B181" s="28" t="s">
         <v>652</v>
       </c>
@@ -9885,7 +9886,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="182" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="182" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B182" s="28" t="s">
         <v>653</v>
       </c>
@@ -9905,7 +9906,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="183" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="183" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B183" s="28" t="s">
         <v>654</v>
       </c>
@@ -9925,7 +9926,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="184" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="184" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B184" t="s">
         <v>655</v>
       </c>
@@ -9955,7 +9956,7 @@
       <c r="AD184" s="26"/>
       <c r="AE184" s="26"/>
     </row>
-    <row r="185" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="185" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B185" s="27" t="s">
         <v>656</v>
       </c>
@@ -9975,7 +9976,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="186" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="186" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B186" s="27" t="s">
         <v>657</v>
       </c>
@@ -9995,7 +9996,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="187" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="187" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B187" s="27" t="s">
         <v>658</v>
       </c>
@@ -10021,7 +10022,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="188" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="188" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B188" s="27" t="s">
         <v>659</v>
       </c>
@@ -10041,7 +10042,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="189" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="189" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B189" s="27" t="s">
         <v>660</v>
       </c>
@@ -10061,7 +10062,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="190" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="190" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B190" s="27" t="s">
         <v>661</v>
       </c>
@@ -10087,7 +10088,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="191" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="191" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B191" s="27" t="s">
         <v>662</v>
       </c>
@@ -10113,7 +10114,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="192" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="192" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B192" s="27" t="s">
         <v>663</v>
       </c>
@@ -10133,7 +10134,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="193" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="193" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B193" s="27" t="s">
         <v>664</v>
       </c>
@@ -10153,7 +10154,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="194" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="194" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B194" s="27" t="s">
         <v>665</v>
       </c>
@@ -10179,7 +10180,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="195" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="195" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B195" s="27" t="s">
         <v>666</v>
       </c>
@@ -10202,7 +10203,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="196" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B196" s="27" t="s">
         <v>667</v>
       </c>
@@ -10228,7 +10229,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="197" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="197" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B197" s="27" t="s">
         <v>668</v>
       </c>
@@ -10264,7 +10265,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="198" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="198" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B198" s="27" t="s">
         <v>669</v>
       </c>
@@ -10290,7 +10291,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="199" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="199" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B199" s="27" t="s">
         <v>670</v>
       </c>
@@ -10326,7 +10327,7 @@
         <v>1088</v>
       </c>
     </row>
-    <row r="200" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="200" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B200" s="27" t="s">
         <v>671</v>
       </c>
@@ -10346,7 +10347,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="201" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="201" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B201" s="27" t="s">
         <v>672</v>
       </c>
@@ -10366,7 +10367,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="202" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="202" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B202" s="27" t="s">
         <v>673</v>
       </c>
@@ -10386,7 +10387,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="203" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="203" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B203" s="27" t="s">
         <v>674</v>
       </c>
@@ -10406,7 +10407,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="204" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="204" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B204" s="27" t="s">
         <v>675</v>
       </c>
@@ -10429,7 +10430,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="205" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="205" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B205" s="27" t="s">
         <v>676</v>
       </c>
@@ -10455,7 +10456,7 @@
         <v>940</v>
       </c>
     </row>
-    <row r="206" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="206" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B206" s="27" t="s">
         <v>282</v>
       </c>
@@ -10475,7 +10476,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="207" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="207" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B207" s="27" t="s">
         <v>677</v>
       </c>
@@ -10495,7 +10496,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="208" spans="2:30" x14ac:dyDescent="0.2">
+    <row r="208" spans="2:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="B208" s="27" t="s">
         <v>678</v>
       </c>
@@ -10521,7 +10522,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="209" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="209" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B209" s="27" t="s">
         <v>679</v>
       </c>
@@ -10547,7 +10548,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="210" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="210" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B210" s="27" t="s">
         <v>680</v>
       </c>
@@ -10567,7 +10568,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="211" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="211" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B211" s="27" t="s">
         <v>681</v>
       </c>
@@ -10587,7 +10588,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="212" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="212" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B212" s="27" t="s">
         <v>682</v>
       </c>
@@ -10607,7 +10608,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="213" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="213" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B213" s="27" t="s">
         <v>683</v>
       </c>
@@ -10627,7 +10628,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="214" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="214" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B214" s="27" t="s">
         <v>684</v>
       </c>
@@ -10653,7 +10654,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="215" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="215" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B215" s="27" t="s">
         <v>685</v>
       </c>
@@ -10673,7 +10674,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="216" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="216" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B216" s="27" t="s">
         <v>686</v>
       </c>
@@ -10693,7 +10694,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="217" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="217" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B217" s="27" t="s">
         <v>687</v>
       </c>
@@ -10713,7 +10714,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="218" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="218" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B218" s="27" t="s">
         <v>688</v>
       </c>
@@ -10733,7 +10734,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="219" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="219" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B219" s="27" t="s">
         <v>689</v>
       </c>
@@ -10759,7 +10760,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="220" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="220" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B220" t="s">
         <v>690</v>
       </c>
@@ -10779,7 +10780,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="221" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="221" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B221" s="28" t="s">
         <v>107</v>
       </c>
@@ -10813,7 +10814,7 @@
       </c>
       <c r="AE221" s="26"/>
     </row>
-    <row r="222" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="222" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B222" s="28" t="s">
         <v>108</v>
       </c>
@@ -10843,7 +10844,7 @@
       <c r="AD222" s="26"/>
       <c r="AE222" s="26"/>
     </row>
-    <row r="223" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="223" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B223" s="28" t="s">
         <v>691</v>
       </c>
@@ -10877,7 +10878,7 @@
       </c>
       <c r="AE223" s="26"/>
     </row>
-    <row r="224" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="224" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B224" s="28" t="s">
         <v>692</v>
       </c>
@@ -10908,7 +10909,7 @@
       <c r="AD224" s="26"/>
       <c r="AE224" s="26"/>
     </row>
-    <row r="225" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="225" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B225" s="28" t="s">
         <v>693</v>
       </c>
@@ -10938,7 +10939,7 @@
         <v>911</v>
       </c>
     </row>
-    <row r="226" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="226" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B226" s="28" t="s">
         <v>694</v>
       </c>
@@ -10965,7 +10966,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="227" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="227" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B227" s="34" t="s">
         <v>695</v>
       </c>
@@ -10996,7 +10997,7 @@
       <c r="AD227" s="32"/>
       <c r="AE227" s="32"/>
     </row>
-    <row r="228" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B228" s="28" t="s">
         <v>696</v>
       </c>
@@ -11017,7 +11018,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="229" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="229" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B229" s="28" t="s">
         <v>697</v>
       </c>
@@ -11044,7 +11045,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="230" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="230" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B230" s="28" t="s">
         <v>698</v>
       </c>
@@ -11070,7 +11071,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="231" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="231" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B231" s="28" t="s">
         <v>699</v>
       </c>
@@ -11096,7 +11097,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="232" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="232" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B232" s="28" t="s">
         <v>700</v>
       </c>
@@ -11128,7 +11129,7 @@
         <v>964</v>
       </c>
     </row>
-    <row r="233" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="233" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B233" s="28" t="s">
         <v>701</v>
       </c>
@@ -11160,7 +11161,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="234" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="234" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B234" s="28" t="s">
         <v>966</v>
       </c>
@@ -11192,7 +11193,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="235" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="235" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B235" s="28" t="s">
         <v>803</v>
       </c>
@@ -11212,7 +11213,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="236" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="236" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B236" s="28" t="s">
         <v>704</v>
       </c>
@@ -11232,7 +11233,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="237" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="237" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B237" s="28" t="s">
         <v>705</v>
       </c>
@@ -11252,7 +11253,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="238" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="238" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B238" s="28" t="s">
         <v>706</v>
       </c>
@@ -11272,7 +11273,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="239" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="239" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B239" s="28" t="s">
         <v>707</v>
       </c>
@@ -11307,7 +11308,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="240" spans="2:31" x14ac:dyDescent="0.2">
+    <row r="240" spans="2:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="B240" s="28" t="s">
         <v>901</v>
       </c>
@@ -11330,7 +11331,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="241" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="241" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B241" s="28" t="s">
         <v>902</v>
       </c>
@@ -11350,7 +11351,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="242" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="242" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B242" t="s">
         <v>1102</v>
       </c>
@@ -11367,7 +11368,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="243" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="243" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B243" t="s">
         <v>1103</v>
       </c>
@@ -11384,7 +11385,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="244" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="244" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B244" t="s">
         <v>1128</v>
       </c>
@@ -11401,7 +11402,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="245" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="245" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B245" t="s">
         <v>1129</v>
       </c>
@@ -11418,7 +11419,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="246" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="246" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B246" t="s">
         <v>708</v>
       </c>
@@ -11438,7 +11439,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="247" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="247" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B247" t="s">
         <v>709</v>
       </c>
@@ -11458,7 +11459,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="248" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="248" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B248" t="s">
         <v>710</v>
       </c>
@@ -11478,7 +11479,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="249" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="249" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B249" t="s">
         <v>711</v>
       </c>
@@ -11498,7 +11499,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="250" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="250" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B250" t="s">
         <v>712</v>
       </c>
@@ -11518,7 +11519,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="251" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="251" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B251" t="s">
         <v>713</v>
       </c>
@@ -11538,7 +11539,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="252" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="252" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B252" t="s">
         <v>714</v>
       </c>
@@ -11558,7 +11559,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="253" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="253" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B253" t="s">
         <v>715</v>
       </c>
@@ -11578,7 +11579,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="254" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="254" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B254" t="s">
         <v>716</v>
       </c>
@@ -11598,7 +11599,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="255" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="255" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B255" t="s">
         <v>717</v>
       </c>
@@ -11618,7 +11619,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="256" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="256" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B256" t="s">
         <v>718</v>
       </c>
@@ -11638,7 +11639,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="257" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="257" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B257" t="s">
         <v>383</v>
       </c>
@@ -11658,7 +11659,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="258" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="258" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B258" t="s">
         <v>384</v>
       </c>
@@ -11678,7 +11679,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="259" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="259" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B259" t="s">
         <v>719</v>
       </c>
@@ -11698,7 +11699,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="260" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="260" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B260" t="s">
         <v>720</v>
       </c>
@@ -11718,7 +11719,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="261" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="261" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B261" t="s">
         <v>721</v>
       </c>
@@ -11738,7 +11739,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="262" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="262" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B262" t="s">
         <v>722</v>
       </c>
@@ -11758,7 +11759,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="263" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="263" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B263" t="s">
         <v>723</v>
       </c>
@@ -11778,7 +11779,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="264" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="264" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B264" t="s">
         <v>724</v>
       </c>
@@ -11798,7 +11799,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="265" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="265" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B265" t="s">
         <v>725</v>
       </c>
@@ -11818,7 +11819,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="266" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="266" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B266" t="s">
         <v>726</v>
       </c>
@@ -11838,7 +11839,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="267" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="267" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B267" t="s">
         <v>727</v>
       </c>
@@ -11858,7 +11859,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="268" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="268" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B268" t="s">
         <v>728</v>
       </c>
@@ -11878,7 +11879,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="269" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="269" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B269" t="s">
         <v>729</v>
       </c>
@@ -11898,7 +11899,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="270" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="270" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B270" t="s">
         <v>730</v>
       </c>
@@ -11918,7 +11919,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="271" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="271" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B271" t="s">
         <v>731</v>
       </c>
@@ -11938,7 +11939,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="272" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="272" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B272" t="s">
         <v>1031</v>
       </c>
@@ -11958,7 +11959,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="273" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="273" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B273" t="s">
         <v>732</v>
       </c>
@@ -11978,7 +11979,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="274" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="274" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B274" t="s">
         <v>733</v>
       </c>
@@ -11998,7 +11999,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="275" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="275" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B275" t="s">
         <v>734</v>
       </c>
@@ -12018,7 +12019,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="276" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="276" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B276" t="s">
         <v>735</v>
       </c>
@@ -12038,7 +12039,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="277" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="277" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B277" t="s">
         <v>736</v>
       </c>
@@ -12058,7 +12059,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="278" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="278" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B278" t="s">
         <v>737</v>
       </c>
@@ -12078,7 +12079,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="279" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="279" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B279" t="s">
         <v>738</v>
       </c>
@@ -12098,7 +12099,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="280" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="280" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B280" t="s">
         <v>739</v>
       </c>
@@ -12118,7 +12119,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="281" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="281" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B281" t="s">
         <v>740</v>
       </c>
@@ -12138,7 +12139,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="282" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="282" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B282" t="s">
         <v>741</v>
       </c>
@@ -12158,7 +12159,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="283" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="283" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B283" t="s">
         <v>742</v>
       </c>
@@ -12178,7 +12179,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="284" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="284" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B284" t="s">
         <v>743</v>
       </c>
@@ -12198,7 +12199,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="285" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="285" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B285" t="s">
         <v>744</v>
       </c>
@@ -12218,7 +12219,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="286" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="286" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B286" t="s">
         <v>745</v>
       </c>
@@ -12238,7 +12239,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="287" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="287" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B287" t="s">
         <v>746</v>
       </c>
@@ -12258,7 +12259,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="288" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="288" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B288" t="s">
         <v>747</v>
       </c>
@@ -12278,7 +12279,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="289" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="289" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B289" t="s">
         <v>748</v>
       </c>
@@ -12298,7 +12299,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="290" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="290" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B290" t="s">
         <v>749</v>
       </c>
@@ -12318,7 +12319,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="291" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="291" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B291" t="s">
         <v>385</v>
       </c>
@@ -12338,7 +12339,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="292" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="292" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B292" t="s">
         <v>750</v>
       </c>
@@ -12358,7 +12359,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="293" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="293" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B293" t="s">
         <v>751</v>
       </c>
@@ -12378,7 +12379,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="294" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="294" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B294" t="s">
         <v>386</v>
       </c>
@@ -12398,7 +12399,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="295" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="295" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B295" t="s">
         <v>752</v>
       </c>
@@ -12418,7 +12419,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="296" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="296" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B296" t="s">
         <v>753</v>
       </c>
@@ -12438,7 +12439,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="297" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="297" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B297" t="s">
         <v>754</v>
       </c>
@@ -12458,7 +12459,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="298" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="298" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B298" t="s">
         <v>755</v>
       </c>
@@ -12478,7 +12479,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="299" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="299" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B299" t="s">
         <v>756</v>
       </c>
@@ -12498,7 +12499,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="300" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="300" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B300" t="s">
         <v>757</v>
       </c>
@@ -12518,7 +12519,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="301" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="301" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B301" t="s">
         <v>758</v>
       </c>
@@ -12538,7 +12539,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="302" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="302" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B302" t="s">
         <v>759</v>
       </c>
@@ -12558,7 +12559,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="303" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="303" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B303" t="s">
         <v>760</v>
       </c>
@@ -12578,7 +12579,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="304" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="304" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B304" t="s">
         <v>761</v>
       </c>
@@ -12598,7 +12599,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="305" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="305" spans="2:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="B305" t="s">
         <v>1134</v>
       </c>
@@ -12621,7 +12622,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="306" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="306" spans="2:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="B306" t="s">
         <v>762</v>
       </c>
@@ -12641,7 +12642,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="307" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="307" spans="2:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="B307" t="s">
         <v>1135</v>
       </c>
@@ -12664,7 +12665,7 @@
         <v>1117</v>
       </c>
     </row>
-    <row r="308" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="308" spans="2:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="B308" t="s">
         <v>763</v>
       </c>
@@ -12684,7 +12685,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="309" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="309" spans="2:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="B309" t="s">
         <v>764</v>
       </c>
@@ -12704,7 +12705,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="310" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="310" spans="2:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="B310" t="s">
         <v>387</v>
       </c>
@@ -12724,7 +12725,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="311" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="311" spans="2:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="B311" t="s">
         <v>388</v>
       </c>
@@ -12744,7 +12745,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="312" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="312" spans="2:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="B312" t="s">
         <v>765</v>
       </c>
@@ -12764,7 +12765,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="313" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="313" spans="2:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="B313" t="s">
         <v>766</v>
       </c>
@@ -12784,7 +12785,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="314" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="314" spans="2:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="B314" t="s">
         <v>767</v>
       </c>
@@ -12804,7 +12805,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="315" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="315" spans="2:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="B315" t="s">
         <v>768</v>
       </c>
@@ -12824,7 +12825,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="316" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="316" spans="2:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="B316" t="s">
         <v>389</v>
       </c>
@@ -12844,7 +12845,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="317" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="317" spans="2:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="B317" t="s">
         <v>769</v>
       </c>
@@ -12864,7 +12865,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="318" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="318" spans="2:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="B318" t="s">
         <v>770</v>
       </c>
@@ -12884,7 +12885,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="319" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="319" spans="2:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="B319" t="s">
         <v>771</v>
       </c>
@@ -12904,7 +12905,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="320" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="320" spans="2:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="B320" t="s">
         <v>772</v>
       </c>
@@ -12924,7 +12925,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="321" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="321" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B321" t="s">
         <v>773</v>
       </c>
@@ -12944,7 +12945,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="322" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="322" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B322" t="s">
         <v>774</v>
       </c>
@@ -12964,7 +12965,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="323" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="323" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B323" t="s">
         <v>775</v>
       </c>
@@ -12984,7 +12985,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="324" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="324" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B324" t="s">
         <v>1032</v>
       </c>
@@ -13004,7 +13005,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="325" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="325" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B325" t="s">
         <v>390</v>
       </c>
@@ -13024,7 +13025,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="326" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="326" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B326" t="s">
         <v>776</v>
       </c>
@@ -13044,7 +13045,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="327" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="327" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B327" t="s">
         <v>777</v>
       </c>
@@ -13064,7 +13065,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="328" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="328" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B328" t="s">
         <v>778</v>
       </c>
@@ -13084,7 +13085,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="329" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="329" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B329" t="s">
         <v>779</v>
       </c>
@@ -13104,7 +13105,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="330" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="330" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B330" t="s">
         <v>780</v>
       </c>
@@ -13124,7 +13125,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="331" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="331" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B331" t="s">
         <v>781</v>
       </c>
@@ -13144,7 +13145,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="332" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="332" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B332" t="s">
         <v>782</v>
       </c>
@@ -13164,7 +13165,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="333" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="333" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B333" t="s">
         <v>783</v>
       </c>
@@ -13184,7 +13185,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="334" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="334" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B334" t="s">
         <v>784</v>
       </c>
@@ -13204,7 +13205,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="335" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="335" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B335" t="s">
         <v>785</v>
       </c>
@@ -13224,7 +13225,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="336" spans="2:9" x14ac:dyDescent="0.2">
+    <row r="336" spans="2:9" hidden="1" x14ac:dyDescent="0.2">
       <c r="B336" t="s">
         <v>786</v>
       </c>
@@ -13244,7 +13245,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="337" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="337" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B337" t="s">
         <v>787</v>
       </c>
@@ -13264,7 +13265,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="338" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="338" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B338" t="s">
         <v>788</v>
       </c>
@@ -13284,7 +13285,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="339" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="339" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B339" t="s">
         <v>789</v>
       </c>
@@ -13304,7 +13305,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="340" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="340" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B340" t="s">
         <v>790</v>
       </c>
@@ -13324,7 +13325,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="341" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="341" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B341" t="s">
         <v>791</v>
       </c>
@@ -13344,7 +13345,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="342" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="342" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B342" t="s">
         <v>792</v>
       </c>
@@ -13364,7 +13365,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="343" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="343" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B343" t="s">
         <v>793</v>
       </c>
@@ -13390,7 +13391,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="344" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="344" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B344" t="s">
         <v>391</v>
       </c>
@@ -13416,7 +13417,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="345" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="345" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B345" t="s">
         <v>392</v>
       </c>
@@ -13436,7 +13437,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="346" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="346" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B346" t="s">
         <v>794</v>
       </c>
@@ -13462,7 +13463,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="347" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="347" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B347" t="s">
         <v>795</v>
       </c>
@@ -13482,7 +13483,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="348" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="348" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B348" t="s">
         <v>796</v>
       </c>
@@ -13502,7 +13503,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="349" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="349" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B349" t="s">
         <v>797</v>
       </c>
@@ -13522,7 +13523,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="350" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="350" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B350" t="s">
         <v>798</v>
       </c>
@@ -13542,7 +13543,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="351" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="351" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B351" t="s">
         <v>799</v>
       </c>
@@ -13568,7 +13569,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="352" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="352" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B352" t="s">
         <v>800</v>
       </c>
@@ -13594,7 +13595,7 @@
         <v>1118</v>
       </c>
     </row>
-    <row r="353" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="353" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B353" t="s">
         <v>801</v>
       </c>
@@ -13614,7 +13615,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="354" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="354" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B354" t="s">
         <v>802</v>
       </c>
@@ -13634,7 +13635,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="355" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="355" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B355" t="s">
         <v>1146</v>
       </c>
@@ -13648,7 +13649,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="356" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="356" spans="2:11" hidden="1" x14ac:dyDescent="0.2">
       <c r="B356" t="s">
         <v>1165</v>
       </c>
@@ -13668,8 +13669,1123 @@
       <c r="J356" s="26"/>
       <c r="K356" s="26"/>
     </row>
+    <row r="357" spans="2:11" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="358" spans="2:11" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="359" spans="2:11" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="360" spans="2:11" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="361" spans="2:11" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="362" spans="2:11" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="363" spans="2:11" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="364" spans="2:11" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="365" spans="2:11" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="366" spans="2:11" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="367" spans="2:11" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="368" spans="2:11" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="369" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="370" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="371" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="372" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="373" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="374" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="375" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="376" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="377" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="378" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="379" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="380" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="381" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="382" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="383" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="384" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="385" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="386" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="387" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="388" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="389" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="390" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="391" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="392" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="393" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="394" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="395" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="396" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="397" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="398" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="399" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="400" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="401" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="402" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="403" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="404" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="405" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="406" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="407" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="408" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="409" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="410" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="411" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="412" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="413" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="414" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="415" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="416" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="417" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="418" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="419" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="420" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="421" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="422" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="423" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="424" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="425" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="426" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="427" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="428" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="429" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="430" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="431" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="432" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="433" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="434" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="435" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="436" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="437" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="438" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="439" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="440" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="441" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="442" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="443" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="444" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="445" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="446" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="447" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="448" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="449" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="450" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="451" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="452" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="453" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="454" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="455" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="456" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="457" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="458" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="459" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="460" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="461" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="462" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="463" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="464" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="465" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="466" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="467" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="468" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="469" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="470" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="471" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="472" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="473" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="474" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="475" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="476" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="477" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="478" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="479" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="480" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="481" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="482" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="483" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="484" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="485" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="486" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="487" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="488" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="489" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="490" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="491" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="492" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="493" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="494" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="495" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="496" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="497" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="498" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="499" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="500" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="501" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="502" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="503" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="504" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="505" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="506" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="507" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="508" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="509" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="510" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="511" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="512" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="513" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="514" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="515" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="516" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="517" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="518" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="519" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="520" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="521" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="522" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="523" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="524" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="525" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="526" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="527" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="528" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="529" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="530" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="531" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="532" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="533" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="534" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="535" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="536" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="537" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="538" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="539" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="540" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="541" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="542" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="543" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="544" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="545" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="546" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="547" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="548" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="549" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="550" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="551" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="552" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="553" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="554" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="555" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="556" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="557" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="558" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="559" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="560" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="561" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="562" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="563" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="564" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="565" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="566" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="567" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="568" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="569" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="570" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="571" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="572" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="573" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="574" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="575" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="576" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="577" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="578" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="579" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="580" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="581" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="582" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="583" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="584" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="585" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="586" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="587" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="588" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="589" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="590" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="591" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="592" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="593" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="594" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="595" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="596" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="597" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="598" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="599" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="600" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="601" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="602" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="603" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="604" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="605" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="606" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="607" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="608" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="609" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="610" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="611" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="612" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="613" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="614" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="615" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="616" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="617" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="618" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="619" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="620" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="621" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="622" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="623" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="624" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="625" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="626" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="627" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="628" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="629" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="630" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="631" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="632" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="633" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="634" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="635" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="636" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="637" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="638" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="639" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="640" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="641" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="642" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="643" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="644" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="645" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="646" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="647" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="648" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="649" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="650" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="651" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="652" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="653" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="654" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="655" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="656" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="657" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="658" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="659" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="660" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="661" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="662" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="663" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="664" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="665" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="666" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="667" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="668" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="669" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="670" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="671" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="672" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="673" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="674" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="675" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="676" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="677" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="678" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="679" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="680" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="681" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="682" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="683" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="684" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="685" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="686" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="687" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="688" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="689" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="690" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="691" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="692" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="693" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="694" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="695" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="696" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="697" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="698" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="699" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="700" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="701" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="702" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="703" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="704" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="705" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="706" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="707" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="708" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="709" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="710" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="711" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="712" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="713" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="714" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="715" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="716" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="717" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="718" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="719" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="720" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="721" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="722" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="723" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="724" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="725" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="726" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="727" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="728" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="729" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="730" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="731" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="732" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="733" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="734" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="735" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="736" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="737" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="738" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="739" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="740" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="741" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="742" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="743" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="744" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="745" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="746" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="747" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="748" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="749" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="750" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="751" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="752" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="753" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="754" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="755" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="756" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="757" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="758" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="759" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="760" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="761" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="762" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="763" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="764" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="765" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="766" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="767" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="768" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="769" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="770" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="771" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="772" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="773" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="774" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="775" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="776" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="777" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="778" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="779" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="780" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="781" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="782" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="783" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="784" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="785" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="786" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="787" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="788" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="789" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="790" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="791" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="792" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="793" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="794" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="795" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="796" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="797" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="798" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="799" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="800" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="801" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="802" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="803" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="804" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="805" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="806" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="807" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="808" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="809" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="810" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="811" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="812" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="813" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="814" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="815" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="816" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="817" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="818" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="819" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="820" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="821" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="822" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="823" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="824" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="825" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="826" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="827" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="828" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="829" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="830" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="831" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="832" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="833" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="834" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="835" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="836" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="837" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="838" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="839" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="840" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="841" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="842" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="843" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="844" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="845" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="846" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="847" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="848" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="849" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="850" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="851" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="852" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="853" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="854" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="855" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="856" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="857" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="858" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="859" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="860" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="861" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="862" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="863" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="864" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="865" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="866" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="867" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="868" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="869" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="870" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="871" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="872" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="873" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="874" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="875" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="876" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="877" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="878" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="879" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="880" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="881" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="882" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="883" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="884" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="885" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="886" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="887" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="888" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="889" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="890" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="891" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="892" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="893" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="894" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="895" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="896" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="897" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="898" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="899" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="900" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="901" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="902" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="903" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="904" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="905" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="906" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="907" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="908" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="909" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="910" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="911" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="912" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="913" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="914" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="915" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="916" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="917" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="918" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="919" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="920" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="921" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="922" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="923" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="924" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="925" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="926" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="927" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="928" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="929" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="930" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="931" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="932" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="933" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="934" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="935" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="936" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="937" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="938" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="939" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="940" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="941" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="942" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="943" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="944" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="945" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="946" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="947" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="948" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="949" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="950" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="951" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="952" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="953" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="954" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="955" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="956" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="957" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="958" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="959" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="960" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="961" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="962" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="963" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="964" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="965" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="966" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="967" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="968" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="969" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="970" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="971" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="972" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="973" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="974" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="975" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="976" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="977" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="978" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="979" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="980" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="981" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="982" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="983" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="984" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="985" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="986" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="987" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="988" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="989" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="990" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="991" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="992" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="993" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="994" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="995" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="996" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="997" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="998" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="999" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1000" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1001" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1002" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1003" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1004" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1005" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1006" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1007" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1008" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1009" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1010" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1011" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1012" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1013" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1014" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1015" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1016" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1017" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1018" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1019" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1020" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1021" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1022" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1023" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1024" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1025" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1026" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1027" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1028" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1029" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1030" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1031" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1032" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1033" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1034" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1035" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1036" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1037" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1038" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1039" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1040" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1041" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1042" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1043" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1044" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1045" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1046" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1047" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1048" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1049" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1050" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1051" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1052" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1053" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1054" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1055" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1056" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1057" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1058" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1059" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1060" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1061" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1062" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1063" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1064" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1065" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1066" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1067" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1068" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1069" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1070" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1071" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1072" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1073" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1074" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1075" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1076" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1077" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1078" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1079" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1080" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1081" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1082" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1083" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1084" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1085" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1086" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1087" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1088" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1089" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1090" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1091" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1092" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1093" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1094" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1095" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1096" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1097" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1098" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1099" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1100" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1101" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1102" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1103" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1104" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1105" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1106" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1107" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1108" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1109" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1110" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1111" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1112" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1113" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1114" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1115" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1116" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1117" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1118" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1119" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1120" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1121" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1122" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1123" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1124" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1125" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1126" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1127" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1128" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1129" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1130" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1131" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1132" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1133" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1134" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1135" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1136" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1137" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1138" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1139" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1140" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1141" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1142" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1143" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1144" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1145" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1146" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1147" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1148" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1149" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1150" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1151" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1152" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1153" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1154" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1155" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1156" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1157" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1158" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1159" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1160" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1161" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1162" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1163" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1164" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1165" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1166" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1167" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1168" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1169" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1170" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1171" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1172" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1173" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1174" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1175" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1176" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1177" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1178" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1179" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1180" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1181" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1182" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1183" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1184" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1185" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1186" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1187" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1188" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1189" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1190" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1191" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1192" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1193" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1194" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1195" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1196" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1197" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1198" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1199" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1200" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1201" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1202" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1203" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1204" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1205" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1206" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1207" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1208" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1209" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1210" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1211" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1212" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1213" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1214" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1215" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1216" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1217" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1218" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1219" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1220" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1221" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1222" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1223" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1224" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1225" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1226" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1227" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1228" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1229" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1230" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1231" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1232" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1233" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1234" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1235" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1236" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1237" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1238" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1239" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1240" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1241" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1242" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1243" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1244" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1245" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1246" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1247" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1248" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1249" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1250" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1251" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1252" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1253" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1254" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1255" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1256" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1257" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1258" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1259" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1260" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1261" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1262" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1263" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1264" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1265" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1266" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1267" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1268" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1269" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1270" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1271" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1272" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1273" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1274" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1275" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1276" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1277" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1278" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1279" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1280" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1281" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1282" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1283" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1284" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1285" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1286" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1287" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1288" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1289" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1290" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1291" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1292" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1293" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1294" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1295" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1296" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1297" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1298" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1299" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1300" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1301" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1302" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1303" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1304" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1305" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1306" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1307" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1308" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1309" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1310" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1311" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1312" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1313" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1314" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1315" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1316" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1317" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1318" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1319" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1320" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1321" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1322" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1323" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1324" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1325" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1326" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1327" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1328" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1329" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1330" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1331" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1332" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1333" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1334" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1335" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1336" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1337" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1338" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1339" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1340" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1341" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1342" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1343" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1344" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1345" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1346" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1347" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1348" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1349" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1350" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1351" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1352" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1353" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1354" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1355" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1356" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1357" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1358" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1359" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1360" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1361" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1362" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1363" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1364" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1365" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1366" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1367" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1368" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1369" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1370" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1371" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1372" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1373" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1374" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1375" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1376" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1377" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1378" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1379" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1380" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1381" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1382" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1383" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1384" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1385" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1386" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1387" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1388" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1389" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1390" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1391" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1392" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1393" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1394" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1395" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1396" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1397" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1398" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1399" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1400" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1401" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1402" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1403" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1404" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1405" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1406" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1407" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1408" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1409" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1410" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1411" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1412" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1413" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1414" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1415" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1416" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1417" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1418" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1419" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1420" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1421" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1422" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1423" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1424" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1425" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1426" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1427" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1428" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1429" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1430" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1431" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1432" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1433" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1434" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1435" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1436" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1437" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1438" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1439" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1440" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1441" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1442" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1443" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1444" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1445" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1446" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1447" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1448" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1449" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1450" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1451" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1452" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1453" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1454" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1455" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1456" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1457" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1458" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1459" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1460" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1461" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1462" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1463" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1464" hidden="1" x14ac:dyDescent="0.2"/>
+    <row r="1465" hidden="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <autoFilter ref="A1:AE1465"/>
+  <autoFilter ref="A1:AE1465">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="hazmatflag"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="F129:F141 F144">
     <cfRule type="duplicateValues" dxfId="10" priority="6"/>
@@ -13958,13 +15074,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z598"/>
+  <dimension ref="A1:Z599"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19668,7 +20784,7 @@
         <v>1102</v>
       </c>
     </row>
-    <row r="593" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="593" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C593" t="s">
         <v>1092</v>
       </c>
@@ -19676,7 +20792,7 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="594" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="594" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C594" t="s">
         <v>1092</v>
       </c>
@@ -19684,7 +20800,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="595" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="595" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C595" t="s">
         <v>1108</v>
       </c>
@@ -19692,7 +20808,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="596" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="596" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C596" t="s">
         <v>1109</v>
       </c>
@@ -19700,7 +20816,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="597" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="597" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C597" t="s">
         <v>1110</v>
       </c>
@@ -19708,7 +20824,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="598" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="598" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C598" t="s">
         <v>1111</v>
       </c>
@@ -19716,12 +20832,16 @@
         <v>103</v>
       </c>
     </row>
+    <row r="599" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B599" t="s">
+        <v>94</v>
+      </c>
+      <c r="D599" s="28" t="s">
+        <v>901</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:Z598">
-    <sortState ref="A2:Z598">
-      <sortCondition descending="1" ref="B1:B598"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:Z598"/>
   <conditionalFormatting sqref="D160">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Digital asset model revised and fixed some duplicate issues
</commit_message>
<xml_diff>
--- a/jcp-dmd/Base Data Model.xlsx
+++ b/jcp-dmd/Base Data Model.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikhilbhatia/jsonconvertor/DMDJCP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shyam.potta/rdp-sourcecode/dataplatform-sampledata/jcp-dmd/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="29440" windowHeight="14420" tabRatio="500" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19640" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="HELP" sheetId="1" r:id="rId1"/>
@@ -31,22 +31,22 @@
     <definedName name="_Attribute_Name">'[1]S7 - Attribute'!$E$2:$E$1048576</definedName>
     <definedName name="_Boolean">'[1]20170320 065838_DataModel_Templ'!#REF!</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">ATTRIBUTES!$A$1:$AE$236</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'E-A-R-C MODEL'!$A$1:$AA$484</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'E-A-R-C MODEL'!$A$1:$AA$549</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">ENTITIES!$A$1:$D$1</definedName>
     <definedName name="_RefDataAttribute">ATTRIBUTES!#REF!</definedName>
     <definedName name="RefDataAttribute">ATTRIBUTES!$E$11:$E$12</definedName>
     <definedName name="Z_BF8E1B46_AD75_6E4F_85B7_6E6C75F2AAA2_.wvu.FilterData" localSheetId="3" hidden="1">ATTRIBUTES!$A$1:$AE$236</definedName>
-    <definedName name="Z_BF8E1B46_AD75_6E4F_85B7_6E6C75F2AAA2_.wvu.FilterData" localSheetId="5" hidden="1">'E-A-R-C MODEL'!$A$1:$AA$470</definedName>
+    <definedName name="Z_BF8E1B46_AD75_6E4F_85B7_6E6C75F2AAA2_.wvu.FilterData" localSheetId="5" hidden="1">'E-A-R-C MODEL'!$A$1:$AA$469</definedName>
     <definedName name="Z_BF8E1B46_AD75_6E4F_85B7_6E6C75F2AAA2_.wvu.FilterData" localSheetId="2" hidden="1">ENTITIES!$A$1:$D$1</definedName>
-    <definedName name="Z_BF8E1B46_AD75_6E4F_85B7_6E6C75F2AAA2_.wvu.Rows" localSheetId="5" hidden="1">'E-A-R-C MODEL'!$471:$471,'E-A-R-C MODEL'!$480:$482</definedName>
+    <definedName name="Z_BF8E1B46_AD75_6E4F_85B7_6E6C75F2AAA2_.wvu.Rows" localSheetId="5" hidden="1">'E-A-R-C MODEL'!$470:$470,'E-A-R-C MODEL'!$479:$481</definedName>
     <definedName name="Z_F59B42B5_12A6_408C_8984_297F5E3274B0_.wvu.FilterData" localSheetId="3" hidden="1">ATTRIBUTES!$A$1:$AE$236</definedName>
-    <definedName name="Z_F59B42B5_12A6_408C_8984_297F5E3274B0_.wvu.FilterData" localSheetId="5" hidden="1">'E-A-R-C MODEL'!$A$1:$AA$470</definedName>
+    <definedName name="Z_F59B42B5_12A6_408C_8984_297F5E3274B0_.wvu.FilterData" localSheetId="5" hidden="1">'E-A-R-C MODEL'!$A$1:$AA$469</definedName>
     <definedName name="Z_F59B42B5_12A6_408C_8984_297F5E3274B0_.wvu.FilterData" localSheetId="2" hidden="1">ENTITIES!$A$1:$D$1</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Microsoft Office User - Personal View" guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" mergeInterval="0" personalView="1" windowWidth="1472" windowHeight="548" tabRatio="500" activeSheetId="4"/>
     <customWorkbookView name="Gupta, Kunal - Personal View" guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" tabRatio="500" activeSheetId="4"/>
-    <customWorkbookView name="Microsoft Office User - Personal View" guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" mergeInterval="0" personalView="1" windowWidth="1472" windowHeight="548" tabRatio="500" activeSheetId="4"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3250" uniqueCount="927">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3540" uniqueCount="976">
   <si>
     <t>ACTION</t>
   </si>
@@ -2917,6 +2917,153 @@
   </si>
   <si>
     <t>PIM</t>
+  </si>
+  <si>
+    <t>colorname</t>
+  </si>
+  <si>
+    <t>Asset Information</t>
+  </si>
+  <si>
+    <t>Color Name</t>
+  </si>
+  <si>
+    <t>colorprofile</t>
+  </si>
+  <si>
+    <t>Color Profile</t>
+  </si>
+  <si>
+    <t>imageformat</t>
+  </si>
+  <si>
+    <t>Image Format</t>
+  </si>
+  <si>
+    <t>imageformatvalues</t>
+  </si>
+  <si>
+    <t>imageheightunit</t>
+  </si>
+  <si>
+    <t>Image Height</t>
+  </si>
+  <si>
+    <t>imageresolution</t>
+  </si>
+  <si>
+    <t>Image Resolution</t>
+  </si>
+  <si>
+    <t>imagesequencing</t>
+  </si>
+  <si>
+    <t>Image Sequencing</t>
+  </si>
+  <si>
+    <t>imagesize</t>
+  </si>
+  <si>
+    <t>Image Size</t>
+  </si>
+  <si>
+    <t>imagetype</t>
+  </si>
+  <si>
+    <t>Image Type</t>
+  </si>
+  <si>
+    <t>imagetypevalues</t>
+  </si>
+  <si>
+    <t>imagewidthunit</t>
+  </si>
+  <si>
+    <t>Image Width</t>
+  </si>
+  <si>
+    <t>lastaccesseddate</t>
+  </si>
+  <si>
+    <t>Last Accessed Date</t>
+  </si>
+  <si>
+    <t>lastmodifieddate</t>
+  </si>
+  <si>
+    <t>Last Modified Date</t>
+  </si>
+  <si>
+    <t>maximagequality</t>
+  </si>
+  <si>
+    <t>Max Image Quality</t>
+  </si>
+  <si>
+    <t>mediatype</t>
+  </si>
+  <si>
+    <t>Media Type</t>
+  </si>
+  <si>
+    <t>month</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>monthvalues</t>
+  </si>
+  <si>
+    <t>shottype</t>
+  </si>
+  <si>
+    <t>Shot Type/Primary Image indicator</t>
+  </si>
+  <si>
+    <t>shottypevalues</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>skutovideo</t>
+  </si>
+  <si>
+    <t>videos</t>
+  </si>
+  <si>
+    <t>lottovideo</t>
+  </si>
+  <si>
+    <t>productpresentationtovideo</t>
+  </si>
+  <si>
+    <t>ensembletovideo</t>
+  </si>
+  <si>
+    <t>skutodocument</t>
+  </si>
+  <si>
+    <t>document</t>
+  </si>
+  <si>
+    <t>lottodocument</t>
+  </si>
+  <si>
+    <t>productpresentationtodocument</t>
+  </si>
+  <si>
+    <t>ensembletodocument</t>
+  </si>
+  <si>
+    <t>audio</t>
+  </si>
+  <si>
+    <t>video</t>
   </si>
 </sst>
 </file>
@@ -2926,7 +3073,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]General"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2997,6 +3144,13 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -3150,7 +3304,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -3205,6 +3359,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="18">
     <cellStyle name="Excel Built-in Normal" xfId="1"/>
@@ -3226,7 +3381,17 @@
     <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3759,12 +3924,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}">
+      <selection activeCell="A5" sqref="A5"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}">
       <selection activeCell="B34" sqref="B34"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}">
-      <selection activeCell="A5" sqref="A5"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -3935,11 +4100,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -4014,14 +4179,14 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="150">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="150">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="150">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -4031,12 +4196,12 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF236"/>
+  <dimension ref="A1:AF252"/>
   <sheetViews>
     <sheetView zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="1" topLeftCell="A214" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+      <selection pane="bottomLeft" activeCell="A237" sqref="A237:XFD252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10711,12 +10876,384 @@
         <v>912</v>
       </c>
     </row>
+    <row r="237" spans="1:30" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B237" s="41" t="s">
+        <v>927</v>
+      </c>
+      <c r="C237" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="E237" s="41" t="s">
+        <v>928</v>
+      </c>
+      <c r="F237" s="41" t="s">
+        <v>929</v>
+      </c>
+      <c r="G237" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="H237" s="26"/>
+      <c r="I237" s="41" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="238" spans="1:30" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B238" s="41" t="s">
+        <v>930</v>
+      </c>
+      <c r="C238" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="E238" s="41" t="s">
+        <v>928</v>
+      </c>
+      <c r="F238" s="41" t="s">
+        <v>931</v>
+      </c>
+      <c r="G238" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="H238" s="26"/>
+      <c r="I238" s="41" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="239" spans="1:30" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B239" s="41" t="s">
+        <v>932</v>
+      </c>
+      <c r="C239" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E239" s="41" t="s">
+        <v>928</v>
+      </c>
+      <c r="F239" s="41" t="s">
+        <v>933</v>
+      </c>
+      <c r="G239" s="41" t="s">
+        <v>881</v>
+      </c>
+      <c r="H239" s="26"/>
+      <c r="I239" s="41" t="s">
+        <v>934</v>
+      </c>
+      <c r="J239" s="41" t="s">
+        <v>869</v>
+      </c>
+      <c r="K239" s="41" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="240" spans="1:30" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B240" s="41" t="s">
+        <v>935</v>
+      </c>
+      <c r="C240" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E240" s="41" t="s">
+        <v>928</v>
+      </c>
+      <c r="F240" s="41" t="s">
+        <v>936</v>
+      </c>
+      <c r="G240" s="41" t="s">
+        <v>881</v>
+      </c>
+      <c r="H240" s="26"/>
+      <c r="I240" s="41" t="s">
+        <v>799</v>
+      </c>
+      <c r="J240" s="41" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="241" spans="2:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B241" s="41" t="s">
+        <v>937</v>
+      </c>
+      <c r="C241" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="E241" s="41" t="s">
+        <v>928</v>
+      </c>
+      <c r="F241" s="41" t="s">
+        <v>938</v>
+      </c>
+      <c r="G241" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="H241" s="26"/>
+      <c r="I241" s="41" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="242" spans="2:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B242" s="41" t="s">
+        <v>939</v>
+      </c>
+      <c r="C242" s="28" t="s">
+        <v>796</v>
+      </c>
+      <c r="E242" s="41" t="s">
+        <v>928</v>
+      </c>
+      <c r="F242" s="41" t="s">
+        <v>940</v>
+      </c>
+      <c r="G242" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="H242" s="26"/>
+      <c r="I242" s="41" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="243" spans="2:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B243" s="41" t="s">
+        <v>941</v>
+      </c>
+      <c r="C243" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="E243" s="41" t="s">
+        <v>928</v>
+      </c>
+      <c r="F243" s="41" t="s">
+        <v>942</v>
+      </c>
+      <c r="G243" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="H243" s="26"/>
+      <c r="I243" s="41" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="244" spans="2:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B244" s="41" t="s">
+        <v>943</v>
+      </c>
+      <c r="C244" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E244" s="41" t="s">
+        <v>928</v>
+      </c>
+      <c r="F244" s="41" t="s">
+        <v>944</v>
+      </c>
+      <c r="G244" s="41" t="s">
+        <v>881</v>
+      </c>
+      <c r="H244" s="26"/>
+      <c r="I244" s="41" t="s">
+        <v>945</v>
+      </c>
+      <c r="J244" s="41" t="s">
+        <v>869</v>
+      </c>
+      <c r="K244" s="41" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="245" spans="2:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B245" s="41" t="s">
+        <v>946</v>
+      </c>
+      <c r="C245" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E245" s="41" t="s">
+        <v>928</v>
+      </c>
+      <c r="F245" s="41" t="s">
+        <v>947</v>
+      </c>
+      <c r="G245" s="41" t="s">
+        <v>881</v>
+      </c>
+      <c r="H245" s="26"/>
+      <c r="I245" s="41" t="s">
+        <v>799</v>
+      </c>
+      <c r="J245" s="41" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="246" spans="2:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B246" s="41" t="s">
+        <v>948</v>
+      </c>
+      <c r="C246" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="E246" s="41" t="s">
+        <v>928</v>
+      </c>
+      <c r="F246" s="41" t="s">
+        <v>949</v>
+      </c>
+      <c r="G246" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="H246" s="26"/>
+      <c r="I246" s="41" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="247" spans="2:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B247" s="41" t="s">
+        <v>950</v>
+      </c>
+      <c r="C247" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="E247" s="41" t="s">
+        <v>928</v>
+      </c>
+      <c r="F247" s="41" t="s">
+        <v>951</v>
+      </c>
+      <c r="G247" s="41" t="s">
+        <v>41</v>
+      </c>
+      <c r="H247" s="26"/>
+      <c r="I247" s="41" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="248" spans="2:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B248" s="41" t="s">
+        <v>952</v>
+      </c>
+      <c r="C248" s="41" t="s">
+        <v>40</v>
+      </c>
+      <c r="E248" s="41" t="s">
+        <v>928</v>
+      </c>
+      <c r="F248" s="41" t="s">
+        <v>953</v>
+      </c>
+      <c r="G248" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="H248" s="26"/>
+      <c r="I248" s="41" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="249" spans="2:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B249" s="41" t="s">
+        <v>954</v>
+      </c>
+      <c r="C249" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E249" s="41" t="s">
+        <v>928</v>
+      </c>
+      <c r="F249" s="41" t="s">
+        <v>955</v>
+      </c>
+      <c r="G249" s="41" t="s">
+        <v>881</v>
+      </c>
+      <c r="H249" s="26"/>
+      <c r="I249" s="41" t="s">
+        <v>797</v>
+      </c>
+      <c r="J249" s="41" t="s">
+        <v>869</v>
+      </c>
+      <c r="K249" s="41" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="250" spans="2:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B250" s="41" t="s">
+        <v>956</v>
+      </c>
+      <c r="C250" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E250" s="41" t="s">
+        <v>928</v>
+      </c>
+      <c r="F250" s="41" t="s">
+        <v>957</v>
+      </c>
+      <c r="G250" s="41" t="s">
+        <v>881</v>
+      </c>
+      <c r="H250" s="26"/>
+      <c r="I250" s="41" t="s">
+        <v>958</v>
+      </c>
+      <c r="J250" s="41" t="s">
+        <v>869</v>
+      </c>
+      <c r="K250" s="41" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="251" spans="2:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B251" s="41" t="s">
+        <v>959</v>
+      </c>
+      <c r="C251" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E251" s="41" t="s">
+        <v>928</v>
+      </c>
+      <c r="F251" s="41" t="s">
+        <v>960</v>
+      </c>
+      <c r="G251" s="41" t="s">
+        <v>881</v>
+      </c>
+      <c r="H251" s="26"/>
+      <c r="I251" s="41" t="s">
+        <v>961</v>
+      </c>
+      <c r="J251" s="41" t="s">
+        <v>869</v>
+      </c>
+      <c r="K251" s="41" t="s">
+        <v>870</v>
+      </c>
+    </row>
+    <row r="252" spans="2:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B252" s="41" t="s">
+        <v>962</v>
+      </c>
+      <c r="C252" s="28" t="s">
+        <v>796</v>
+      </c>
+      <c r="E252" s="41" t="s">
+        <v>928</v>
+      </c>
+      <c r="F252" s="41" t="s">
+        <v>963</v>
+      </c>
+      <c r="G252" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="H252" s="26"/>
+      <c r="I252" s="41" t="s">
+        <v>799</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AE236"/>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1" topLeftCell="E1">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A318" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B322" sqref="B322"/>
       <colBreaks count="1" manualBreakCount="1">
         <brk id="2" max="1048575" man="1"/>
       </colBreaks>
@@ -10724,9 +11261,9 @@
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A1:AE347"/>
     </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A318" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B322" sqref="B322"/>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1" topLeftCell="E1">
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
       <colBreaks count="1" manualBreakCount="1">
         <brk id="2" max="1048575" man="1"/>
       </colBreaks>
@@ -10737,24 +11274,27 @@
   </customSheetViews>
   <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="F141:F142">
-    <cfRule type="duplicateValues" dxfId="11" priority="3"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F141:F142">
-    <cfRule type="duplicateValues" dxfId="9" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B235">
-    <cfRule type="duplicateValues" dxfId="8" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F128:F140">
-    <cfRule type="duplicateValues" dxfId="7" priority="11"/>
-    <cfRule type="duplicateValues" dxfId="6" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F128:F140">
-    <cfRule type="duplicateValues" dxfId="5" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="14"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1:B234 B236:B1048576">
-    <cfRule type="duplicateValues" dxfId="4" priority="14"/>
+  <conditionalFormatting sqref="B1:B234 B236 B253:B1048576">
+    <cfRule type="duplicateValues" dxfId="5" priority="15"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B237:B252">
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
@@ -10766,11 +11306,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K10"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView zoomScale="107" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11019,16 +11559,184 @@
         <v>864</v>
       </c>
     </row>
+    <row r="11" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="41" t="s">
+        <v>964</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>965</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="G11" s="41" t="s">
+        <v>850</v>
+      </c>
+      <c r="H11" s="41" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="41" t="s">
+        <v>966</v>
+      </c>
+      <c r="C12" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>965</v>
+      </c>
+      <c r="F12" s="10"/>
+      <c r="G12" s="41" t="s">
+        <v>850</v>
+      </c>
+      <c r="H12" s="41" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="41" t="s">
+        <v>967</v>
+      </c>
+      <c r="C13" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>865</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>965</v>
+      </c>
+      <c r="F13" s="10"/>
+      <c r="G13" s="41" t="s">
+        <v>850</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="41" t="s">
+        <v>968</v>
+      </c>
+      <c r="C14" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>965</v>
+      </c>
+      <c r="F14" s="10"/>
+      <c r="G14" s="41" t="s">
+        <v>850</v>
+      </c>
+      <c r="H14" s="41" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="41" t="s">
+        <v>969</v>
+      </c>
+      <c r="C15" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>970</v>
+      </c>
+      <c r="F15" s="10"/>
+      <c r="G15" s="41" t="s">
+        <v>850</v>
+      </c>
+      <c r="H15" s="41" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="41" t="s">
+        <v>971</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="E16" s="41" t="s">
+        <v>970</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="41" t="s">
+        <v>850</v>
+      </c>
+      <c r="H16" s="41" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="41" t="s">
+        <v>972</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>865</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>970</v>
+      </c>
+      <c r="F17" s="10"/>
+      <c r="G17" s="41" t="s">
+        <v>850</v>
+      </c>
+      <c r="H17" s="41" t="s">
+        <v>864</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="41" t="s">
+        <v>973</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="E18" s="41" t="s">
+        <v>970</v>
+      </c>
+      <c r="F18" s="10"/>
+      <c r="G18" s="41" t="s">
+        <v>850</v>
+      </c>
+      <c r="H18" s="41" t="s">
+        <v>864</v>
+      </c>
+    </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="107">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="107">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="107">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -11039,10 +11747,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA484"/>
+  <dimension ref="A1:AA549"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A453" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D459" sqref="D459"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15122,7 +15831,7 @@
         <v>93</v>
       </c>
       <c r="D400" s="28" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="AA400" s="28"/>
     </row>
@@ -15131,7 +15840,7 @@
         <v>93</v>
       </c>
       <c r="D401" s="28" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="AA401" s="28"/>
     </row>
@@ -15140,7 +15849,7 @@
         <v>93</v>
       </c>
       <c r="D402" s="28" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="AA402" s="28"/>
     </row>
@@ -15149,7 +15858,7 @@
         <v>93</v>
       </c>
       <c r="D403" s="28" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="AA403" s="28"/>
     </row>
@@ -15157,47 +15866,52 @@
       <c r="B404" t="s">
         <v>93</v>
       </c>
-      <c r="D404" s="28" t="s">
-        <v>575</v>
-      </c>
-      <c r="AA404" s="28"/>
+      <c r="E404" t="s">
+        <v>861</v>
+      </c>
     </row>
     <row r="405" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B405" t="s">
-        <v>93</v>
-      </c>
-      <c r="E405" t="s">
-        <v>861</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="D405" s="28" t="s">
+        <v>882</v>
+      </c>
+      <c r="E405" s="27"/>
+      <c r="AA405" s="27"/>
     </row>
     <row r="406" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B406" t="s">
         <v>96</v>
       </c>
-      <c r="D406" s="28" t="s">
-        <v>882</v>
-      </c>
-      <c r="E406" s="27"/>
-      <c r="AA406" s="27"/>
+      <c r="D406" t="s">
+        <v>794</v>
+      </c>
+      <c r="F406" t="s">
+        <v>39</v>
+      </c>
+      <c r="J406" t="s">
+        <v>278</v>
+      </c>
+      <c r="O406" t="s">
+        <v>892</v>
+      </c>
+      <c r="AA406" s="27" t="s">
+        <v>631</v>
+      </c>
     </row>
     <row r="407" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B407" t="s">
         <v>96</v>
       </c>
-      <c r="D407" t="s">
-        <v>794</v>
-      </c>
-      <c r="F407" t="s">
-        <v>39</v>
-      </c>
-      <c r="J407" t="s">
-        <v>278</v>
+      <c r="D407" s="27" t="s">
+        <v>379</v>
       </c>
       <c r="O407" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="AA407" s="27" t="s">
-        <v>631</v>
+        <v>586</v>
       </c>
     </row>
     <row r="408" spans="2:27" x14ac:dyDescent="0.2">
@@ -15205,13 +15919,10 @@
         <v>96</v>
       </c>
       <c r="D408" s="27" t="s">
-        <v>379</v>
-      </c>
-      <c r="O408" t="s">
-        <v>891</v>
+        <v>380</v>
       </c>
       <c r="AA408" s="27" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="409" spans="2:27" x14ac:dyDescent="0.2">
@@ -15219,10 +15930,10 @@
         <v>96</v>
       </c>
       <c r="D409" s="27" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AA409" s="27" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
     </row>
     <row r="410" spans="2:27" x14ac:dyDescent="0.2">
@@ -15230,10 +15941,10 @@
         <v>96</v>
       </c>
       <c r="D410" s="27" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AA410" s="27" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
     </row>
     <row r="411" spans="2:27" x14ac:dyDescent="0.2">
@@ -15241,10 +15952,10 @@
         <v>96</v>
       </c>
       <c r="D411" s="27" t="s">
-        <v>382</v>
+        <v>101</v>
       </c>
       <c r="AA411" s="27" t="s">
-        <v>589</v>
+        <v>5</v>
       </c>
     </row>
     <row r="412" spans="2:27" x14ac:dyDescent="0.2">
@@ -15252,10 +15963,10 @@
         <v>96</v>
       </c>
       <c r="D412" s="27" t="s">
-        <v>101</v>
+        <v>493</v>
       </c>
       <c r="AA412" s="27" t="s">
-        <v>5</v>
+        <v>632</v>
       </c>
     </row>
     <row r="413" spans="2:27" x14ac:dyDescent="0.2">
@@ -15263,10 +15974,10 @@
         <v>96</v>
       </c>
       <c r="D413" s="27" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="AA413" s="27" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
     </row>
     <row r="414" spans="2:27" x14ac:dyDescent="0.2">
@@ -15274,10 +15985,10 @@
         <v>96</v>
       </c>
       <c r="D414" s="27" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="AA414" s="27" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
     </row>
     <row r="415" spans="2:27" x14ac:dyDescent="0.2">
@@ -15285,10 +15996,10 @@
         <v>96</v>
       </c>
       <c r="D415" s="27" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="AA415" s="27" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
     </row>
     <row r="416" spans="2:27" x14ac:dyDescent="0.2">
@@ -15296,10 +16007,10 @@
         <v>96</v>
       </c>
       <c r="D416" s="27" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="AA416" s="27" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
     </row>
     <row r="417" spans="2:27" x14ac:dyDescent="0.2">
@@ -15307,10 +16018,10 @@
         <v>96</v>
       </c>
       <c r="D417" s="27" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="AA417" s="27" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
     </row>
     <row r="418" spans="2:27" x14ac:dyDescent="0.2">
@@ -15318,32 +16029,32 @@
         <v>96</v>
       </c>
       <c r="D418" s="27" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="AA418" s="27" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
     </row>
     <row r="419" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B419" t="s">
         <v>96</v>
       </c>
-      <c r="D419" s="27" t="s">
-        <v>499</v>
+      <c r="D419" s="28" t="s">
+        <v>530</v>
       </c>
       <c r="AA419" s="27" t="s">
-        <v>638</v>
+        <v>595</v>
       </c>
     </row>
     <row r="420" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B420" t="s">
         <v>96</v>
       </c>
-      <c r="D420" s="28" t="s">
-        <v>530</v>
+      <c r="D420" s="27" t="s">
+        <v>502</v>
       </c>
       <c r="AA420" s="27" t="s">
-        <v>595</v>
+        <v>641</v>
       </c>
     </row>
     <row r="421" spans="2:27" x14ac:dyDescent="0.2">
@@ -15351,10 +16062,10 @@
         <v>96</v>
       </c>
       <c r="D421" s="27" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="AA421" s="27" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
     </row>
     <row r="422" spans="2:27" x14ac:dyDescent="0.2">
@@ -15362,10 +16073,10 @@
         <v>96</v>
       </c>
       <c r="D422" s="27" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="AA422" s="27" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
     </row>
     <row r="423" spans="2:27" x14ac:dyDescent="0.2">
@@ -15373,10 +16084,10 @@
         <v>96</v>
       </c>
       <c r="D423" s="27" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="AA423" s="27" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="424" spans="2:27" x14ac:dyDescent="0.2">
@@ -15384,10 +16095,10 @@
         <v>96</v>
       </c>
       <c r="D424" s="27" t="s">
-        <v>505</v>
-      </c>
-      <c r="AA424" s="27" t="s">
-        <v>644</v>
+        <v>506</v>
+      </c>
+      <c r="AA424" s="35" t="s">
+        <v>645</v>
       </c>
     </row>
     <row r="425" spans="2:27" x14ac:dyDescent="0.2">
@@ -15395,10 +16106,10 @@
         <v>96</v>
       </c>
       <c r="D425" s="27" t="s">
-        <v>506</v>
-      </c>
-      <c r="AA425" s="35" t="s">
-        <v>645</v>
+        <v>509</v>
+      </c>
+      <c r="AA425" s="27" t="s">
+        <v>648</v>
       </c>
     </row>
     <row r="426" spans="2:27" x14ac:dyDescent="0.2">
@@ -15406,10 +16117,10 @@
         <v>96</v>
       </c>
       <c r="D426" s="27" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="AA426" s="27" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="427" spans="2:27" x14ac:dyDescent="0.2">
@@ -15417,10 +16128,10 @@
         <v>96</v>
       </c>
       <c r="D427" s="27" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="AA427" s="27" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="428" spans="2:27" x14ac:dyDescent="0.2">
@@ -15428,10 +16139,10 @@
         <v>96</v>
       </c>
       <c r="D428" s="27" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="AA428" s="27" t="s">
-        <v>650</v>
+        <v>652</v>
       </c>
     </row>
     <row r="429" spans="2:27" x14ac:dyDescent="0.2">
@@ -15439,10 +16150,10 @@
         <v>96</v>
       </c>
       <c r="D429" s="27" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="AA429" s="27" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
     </row>
     <row r="430" spans="2:27" x14ac:dyDescent="0.2">
@@ -15450,10 +16161,10 @@
         <v>96</v>
       </c>
       <c r="D430" s="27" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="AA430" s="27" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
     </row>
     <row r="431" spans="2:27" x14ac:dyDescent="0.2">
@@ -15461,10 +16172,10 @@
         <v>96</v>
       </c>
       <c r="D431" s="27" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="AA431" s="27" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
     </row>
     <row r="432" spans="2:27" x14ac:dyDescent="0.2">
@@ -15472,10 +16183,10 @@
         <v>96</v>
       </c>
       <c r="D432" s="27" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="AA432" s="27" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
     </row>
     <row r="433" spans="2:27" x14ac:dyDescent="0.2">
@@ -15483,10 +16194,10 @@
         <v>96</v>
       </c>
       <c r="D433" s="27" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="AA433" s="27" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
     </row>
     <row r="434" spans="2:27" x14ac:dyDescent="0.2">
@@ -15494,10 +16205,10 @@
         <v>96</v>
       </c>
       <c r="D434" s="27" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="AA434" s="27" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
     </row>
     <row r="435" spans="2:27" x14ac:dyDescent="0.2">
@@ -15505,32 +16216,32 @@
         <v>96</v>
       </c>
       <c r="D435" s="27" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="AA435" s="27" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
     </row>
     <row r="436" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B436" t="s">
         <v>96</v>
       </c>
-      <c r="D436" s="27" t="s">
-        <v>520</v>
+      <c r="D436" s="28" t="s">
+        <v>549</v>
       </c>
       <c r="AA436" s="27" t="s">
-        <v>659</v>
+        <v>623</v>
       </c>
     </row>
     <row r="437" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B437" t="s">
         <v>96</v>
       </c>
-      <c r="D437" s="28" t="s">
-        <v>549</v>
+      <c r="D437" s="27" t="s">
+        <v>521</v>
       </c>
       <c r="AA437" s="27" t="s">
-        <v>623</v>
+        <v>660</v>
       </c>
     </row>
     <row r="438" spans="2:27" x14ac:dyDescent="0.2">
@@ -15538,10 +16249,10 @@
         <v>96</v>
       </c>
       <c r="D438" s="27" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="AA438" s="27" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
     </row>
     <row r="439" spans="2:27" x14ac:dyDescent="0.2">
@@ -15549,21 +16260,21 @@
         <v>96</v>
       </c>
       <c r="D439" s="27" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="AA439" s="27" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
     </row>
     <row r="440" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B440" t="s">
         <v>96</v>
       </c>
-      <c r="D440" s="27" t="s">
-        <v>523</v>
+      <c r="D440" s="28" t="s">
+        <v>104</v>
       </c>
       <c r="AA440" s="27" t="s">
-        <v>662</v>
+        <v>592</v>
       </c>
     </row>
     <row r="441" spans="2:27" x14ac:dyDescent="0.2">
@@ -15571,21 +16282,19 @@
         <v>96</v>
       </c>
       <c r="D441" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA441" s="27" t="s">
-        <v>592</v>
-      </c>
+        <v>384</v>
+      </c>
+      <c r="N441" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA441" s="27"/>
     </row>
     <row r="442" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B442" t="s">
         <v>96</v>
       </c>
       <c r="D442" s="28" t="s">
-        <v>384</v>
-      </c>
-      <c r="N442" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
       <c r="AA442" s="27"/>
     </row>
@@ -15594,27 +16303,27 @@
         <v>96</v>
       </c>
       <c r="D443" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA443" s="27"/>
+        <v>526</v>
+      </c>
+      <c r="AA443" s="27" t="s">
+        <v>664</v>
+      </c>
     </row>
     <row r="444" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B444" t="s">
         <v>96</v>
       </c>
       <c r="D444" s="28" t="s">
-        <v>526</v>
-      </c>
-      <c r="AA444" s="27" t="s">
-        <v>664</v>
-      </c>
+        <v>527</v>
+      </c>
+      <c r="AA444" s="28"/>
     </row>
     <row r="445" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B445" t="s">
         <v>96</v>
       </c>
       <c r="D445" s="28" t="s">
-        <v>527</v>
+        <v>880</v>
       </c>
       <c r="AA445" s="28"/>
     </row>
@@ -15623,7 +16332,7 @@
         <v>96</v>
       </c>
       <c r="D446" s="28" t="s">
-        <v>880</v>
+        <v>573</v>
       </c>
       <c r="AA446" s="28"/>
     </row>
@@ -15632,7 +16341,7 @@
         <v>96</v>
       </c>
       <c r="D447" s="28" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="AA447" s="28"/>
     </row>
@@ -15641,7 +16350,7 @@
         <v>96</v>
       </c>
       <c r="D448" s="28" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="AA448" s="28"/>
     </row>
@@ -15649,25 +16358,30 @@
       <c r="B449" t="s">
         <v>96</v>
       </c>
-      <c r="D449" s="28" t="s">
-        <v>575</v>
-      </c>
-      <c r="AA449" s="28"/>
+      <c r="E449" t="s">
+        <v>845</v>
+      </c>
     </row>
     <row r="450" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B450" t="s">
         <v>96</v>
       </c>
       <c r="E450" t="s">
-        <v>845</v>
+        <v>863</v>
       </c>
     </row>
     <row r="451" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B451" t="s">
         <v>96</v>
       </c>
-      <c r="E451" t="s">
-        <v>863</v>
+      <c r="D451" s="28" t="s">
+        <v>877</v>
+      </c>
+      <c r="N451" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA451" s="27" t="s">
+        <v>580</v>
       </c>
     </row>
     <row r="452" spans="2:27" x14ac:dyDescent="0.2">
@@ -15675,38 +16389,32 @@
         <v>96</v>
       </c>
       <c r="D452" s="28" t="s">
-        <v>877</v>
-      </c>
-      <c r="N452" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA452" s="27" t="s">
-        <v>580</v>
-      </c>
+        <v>876</v>
+      </c>
+      <c r="AA452" s="27"/>
     </row>
     <row r="453" spans="2:27" x14ac:dyDescent="0.2">
-      <c r="B453" t="s">
-        <v>96</v>
-      </c>
-      <c r="D453" s="28" t="s">
-        <v>876</v>
-      </c>
-      <c r="AA453" s="27"/>
+      <c r="C453" t="s">
+        <v>848</v>
+      </c>
+      <c r="D453" t="s">
+        <v>855</v>
+      </c>
     </row>
     <row r="454" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C454" t="s">
         <v>848</v>
       </c>
       <c r="D454" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
     </row>
     <row r="455" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C455" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="D455" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
     </row>
     <row r="456" spans="2:27" x14ac:dyDescent="0.2">
@@ -15714,7 +16422,7 @@
         <v>844</v>
       </c>
       <c r="D456" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
     </row>
     <row r="457" spans="2:27" x14ac:dyDescent="0.2">
@@ -15722,15 +16430,15 @@
         <v>844</v>
       </c>
       <c r="D457" t="s">
-        <v>856</v>
+        <v>102</v>
       </c>
     </row>
     <row r="458" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C458" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="D458" t="s">
-        <v>102</v>
+        <v>855</v>
       </c>
     </row>
     <row r="459" spans="2:27" x14ac:dyDescent="0.2">
@@ -15738,7 +16446,7 @@
         <v>845</v>
       </c>
       <c r="D459" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
     </row>
     <row r="460" spans="2:27" x14ac:dyDescent="0.2">
@@ -15746,12 +16454,12 @@
         <v>845</v>
       </c>
       <c r="D460" t="s">
-        <v>856</v>
+        <v>102</v>
       </c>
     </row>
     <row r="461" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C461" t="s">
-        <v>845</v>
+        <v>860</v>
       </c>
       <c r="D461" t="s">
         <v>102</v>
@@ -15759,7 +16467,7 @@
     </row>
     <row r="462" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C462" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="D462" t="s">
         <v>102</v>
@@ -15767,7 +16475,7 @@
     </row>
     <row r="463" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C463" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="D463" t="s">
         <v>102</v>
@@ -15775,23 +16483,23 @@
     </row>
     <row r="464" spans="2:27" x14ac:dyDescent="0.2">
       <c r="C464" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="D464" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="465" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C465" t="s">
-        <v>863</v>
+      <c r="B465" t="s">
+        <v>865</v>
       </c>
       <c r="D465" t="s">
-        <v>102</v>
+        <v>415</v>
       </c>
     </row>
     <row r="466" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B466" t="s">
-        <v>865</v>
+        <v>96</v>
       </c>
       <c r="D466" t="s">
         <v>415</v>
@@ -15799,15 +16507,18 @@
     </row>
     <row r="467" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B467" t="s">
-        <v>96</v>
+        <v>30</v>
       </c>
       <c r="D467" t="s">
-        <v>415</v>
+        <v>905</v>
+      </c>
+      <c r="O467" t="s">
+        <v>906</v>
       </c>
     </row>
     <row r="468" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B468" t="s">
-        <v>30</v>
+        <v>93</v>
       </c>
       <c r="D468" t="s">
         <v>905</v>
@@ -15818,29 +16529,29 @@
     </row>
     <row r="469" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B469" t="s">
-        <v>93</v>
+        <v>30</v>
       </c>
       <c r="D469" t="s">
-        <v>905</v>
-      </c>
-      <c r="O469" t="s">
-        <v>906</v>
+        <v>910</v>
       </c>
     </row>
     <row r="470" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B470" t="s">
-        <v>30</v>
+      <c r="C470" t="s">
+        <v>847</v>
       </c>
       <c r="D470" t="s">
-        <v>910</v>
+        <v>559</v>
       </c>
     </row>
     <row r="471" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="C471" t="s">
-        <v>847</v>
+      <c r="B471" t="s">
+        <v>30</v>
       </c>
       <c r="D471" t="s">
-        <v>559</v>
+        <v>876</v>
+      </c>
+      <c r="M471" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="472" spans="2:15" x14ac:dyDescent="0.2">
@@ -15848,9 +16559,9 @@
         <v>30</v>
       </c>
       <c r="D472" t="s">
-        <v>876</v>
-      </c>
-      <c r="M472" t="s">
+        <v>877</v>
+      </c>
+      <c r="N472" t="s">
         <v>39</v>
       </c>
     </row>
@@ -15859,10 +16570,7 @@
         <v>30</v>
       </c>
       <c r="D473" t="s">
-        <v>877</v>
-      </c>
-      <c r="N473" t="s">
-        <v>39</v>
+        <v>523</v>
       </c>
     </row>
     <row r="474" spans="2:15" x14ac:dyDescent="0.2">
@@ -15870,7 +16578,7 @@
         <v>30</v>
       </c>
       <c r="D474" t="s">
-        <v>523</v>
+        <v>562</v>
       </c>
     </row>
     <row r="475" spans="2:15" x14ac:dyDescent="0.2">
@@ -15878,7 +16586,7 @@
         <v>30</v>
       </c>
       <c r="D475" t="s">
-        <v>562</v>
+        <v>569</v>
       </c>
     </row>
     <row r="476" spans="2:15" x14ac:dyDescent="0.2">
@@ -15886,7 +16594,7 @@
         <v>30</v>
       </c>
       <c r="D476" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
     </row>
     <row r="477" spans="2:15" x14ac:dyDescent="0.2">
@@ -15894,23 +16602,23 @@
         <v>30</v>
       </c>
       <c r="D477" t="s">
-        <v>570</v>
+        <v>733</v>
       </c>
     </row>
     <row r="478" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B478" t="s">
         <v>30</v>
       </c>
-      <c r="D478" t="s">
-        <v>733</v>
+      <c r="D478" s="28" t="s">
+        <v>560</v>
       </c>
     </row>
     <row r="479" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B479" t="s">
-        <v>30</v>
-      </c>
-      <c r="D479" s="28" t="s">
-        <v>560</v>
+        <v>93</v>
+      </c>
+      <c r="D479" t="s">
+        <v>876</v>
       </c>
     </row>
     <row r="480" spans="2:15" x14ac:dyDescent="0.2">
@@ -15918,31 +16626,34 @@
         <v>93</v>
       </c>
       <c r="D480" t="s">
-        <v>876</v>
-      </c>
-    </row>
-    <row r="481" spans="2:15" x14ac:dyDescent="0.2">
+        <v>877</v>
+      </c>
+      <c r="N480" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="481" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B481" t="s">
         <v>93</v>
       </c>
       <c r="D481" t="s">
-        <v>877</v>
-      </c>
-      <c r="N481" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="482" spans="2:15" x14ac:dyDescent="0.2">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="482" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B482" t="s">
-        <v>93</v>
-      </c>
-      <c r="D482" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="483" spans="2:15" x14ac:dyDescent="0.2">
+        <v>865</v>
+      </c>
+      <c r="D482" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="O482" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="483" spans="2:27" x14ac:dyDescent="0.2">
       <c r="B483" t="s">
-        <v>865</v>
+        <v>96</v>
       </c>
       <c r="D483" s="28" t="s">
         <v>109</v>
@@ -15951,26 +16662,551 @@
         <v>926</v>
       </c>
     </row>
-    <row r="484" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B484" t="s">
+    <row r="484" spans="2:27" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B484" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D484" s="41" t="s">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="485" spans="2:27" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B485" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D485" s="41" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="486" spans="2:27" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B486" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D486" s="41" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="487" spans="2:27" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B487" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D487" s="41" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="488" spans="2:27" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B488" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D488" s="41" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="489" spans="2:27" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B489" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D489" s="41" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="490" spans="2:27" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B490" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D490" s="41" t="s">
+        <v>937</v>
+      </c>
+    </row>
+    <row r="491" spans="2:27" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B491" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D491" s="41" t="s">
+        <v>941</v>
+      </c>
+    </row>
+    <row r="492" spans="2:27" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B492" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D492" s="41" t="s">
+        <v>943</v>
+      </c>
+    </row>
+    <row r="493" spans="2:27" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B493" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D493" s="41" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="494" spans="2:27" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B494" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D494" s="41" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="495" spans="2:27" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B495" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D495" s="41" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="496" spans="2:27" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B496" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D496" s="28" t="s">
+        <v>882</v>
+      </c>
+      <c r="E496" s="27"/>
+      <c r="AA496" s="27"/>
+    </row>
+    <row r="497" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B497" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D497" s="41" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="498" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B498" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D498" s="41" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="499" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B499" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D499" s="41" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="500" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B500" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D500" s="41" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="501" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B501" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D501" s="41" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="502" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B502" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D502" s="41" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="503" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B503" s="41" t="s">
+        <v>375</v>
+      </c>
+      <c r="D503" s="41" t="s">
+        <v>402</v>
+      </c>
+      <c r="O503" s="41" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="504" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B504" s="41" t="s">
+        <v>970</v>
+      </c>
+      <c r="D504" s="41" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="505" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B505" s="41" t="s">
+        <v>970</v>
+      </c>
+      <c r="D505" s="41" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="506" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B506" s="41" t="s">
+        <v>970</v>
+      </c>
+      <c r="D506" s="41" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="507" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B507" s="41" t="s">
+        <v>970</v>
+      </c>
+      <c r="D507" s="41" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="508" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B508" s="41" t="s">
+        <v>970</v>
+      </c>
+      <c r="D508" s="28" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="509" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B509" s="41" t="s">
+        <v>970</v>
+      </c>
+      <c r="D509" s="41" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="510" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B510" s="41" t="s">
+        <v>970</v>
+      </c>
+      <c r="D510" s="41" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="511" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B511" s="41" t="s">
+        <v>970</v>
+      </c>
+      <c r="D511" s="41" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="512" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B512" s="41" t="s">
+        <v>970</v>
+      </c>
+      <c r="D512" s="41" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="513" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B513" s="41" t="s">
+        <v>970</v>
+      </c>
+      <c r="D513" s="41" t="s">
+        <v>402</v>
+      </c>
+      <c r="O513" s="41" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="514" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B514" s="41" t="s">
+        <v>974</v>
+      </c>
+      <c r="D514" s="41" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="515" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B515" s="41" t="s">
+        <v>974</v>
+      </c>
+      <c r="D515" s="41" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="516" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B516" s="41" t="s">
+        <v>974</v>
+      </c>
+      <c r="D516" s="41" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="517" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B517" s="41" t="s">
+        <v>974</v>
+      </c>
+      <c r="D517" s="41" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="518" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B518" s="41" t="s">
+        <v>974</v>
+      </c>
+      <c r="D518" s="28" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="519" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B519" s="41" t="s">
+        <v>974</v>
+      </c>
+      <c r="D519" s="41" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="520" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B520" s="41" t="s">
+        <v>974</v>
+      </c>
+      <c r="D520" s="41" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="521" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B521" s="41" t="s">
+        <v>974</v>
+      </c>
+      <c r="D521" s="41" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="522" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B522" s="41" t="s">
+        <v>974</v>
+      </c>
+      <c r="D522" s="41" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="523" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B523" s="41" t="s">
+        <v>974</v>
+      </c>
+      <c r="D523" s="41" t="s">
+        <v>402</v>
+      </c>
+      <c r="O523" s="41" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="524" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B524" s="41" t="s">
+        <v>975</v>
+      </c>
+      <c r="D524" s="41" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="525" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B525" s="41" t="s">
+        <v>975</v>
+      </c>
+      <c r="D525" s="41" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="526" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B526" s="41" t="s">
+        <v>975</v>
+      </c>
+      <c r="D526" s="41" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="527" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B527" s="41" t="s">
+        <v>975</v>
+      </c>
+      <c r="D527" s="41" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="528" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B528" s="41" t="s">
+        <v>975</v>
+      </c>
+      <c r="D528" s="28" t="s">
+        <v>882</v>
+      </c>
+    </row>
+    <row r="529" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B529" s="41" t="s">
+        <v>975</v>
+      </c>
+      <c r="D529" s="41" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="530" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B530" s="41" t="s">
+        <v>975</v>
+      </c>
+      <c r="D530" s="41" t="s">
+        <v>959</v>
+      </c>
+    </row>
+    <row r="531" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B531" s="41" t="s">
+        <v>975</v>
+      </c>
+      <c r="D531" s="41" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="532" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B532" s="41" t="s">
+        <v>975</v>
+      </c>
+      <c r="D532" s="41" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="533" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B533" s="41" t="s">
+        <v>975</v>
+      </c>
+      <c r="D533" s="41" t="s">
+        <v>402</v>
+      </c>
+      <c r="O533" s="41" t="s">
+        <v>904</v>
+      </c>
+    </row>
+    <row r="534" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B534" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="E534" s="41" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="535" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B535" s="41" t="s">
+        <v>865</v>
+      </c>
+      <c r="E535" s="41" t="s">
+        <v>971</v>
+      </c>
+    </row>
+    <row r="536" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B536" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="E536" s="41" t="s">
+        <v>972</v>
+      </c>
+    </row>
+    <row r="537" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B537" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="D484" s="28" t="s">
-        <v>109</v>
-      </c>
-      <c r="O484" t="s">
-        <v>926</v>
+      <c r="E537" s="41" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="538" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B538" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="E538" s="41" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="539" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B539" s="41" t="s">
+        <v>865</v>
+      </c>
+      <c r="E539" s="41" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="540" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B540" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="E540" s="41" t="s">
+        <v>967</v>
+      </c>
+    </row>
+    <row r="541" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B541" s="41" t="s">
+        <v>96</v>
+      </c>
+      <c r="E541" s="41" t="s">
+        <v>968</v>
+      </c>
+    </row>
+    <row r="542" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C542" s="42" t="s">
+        <v>969</v>
+      </c>
+      <c r="D542" s="41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="543" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C543" s="42" t="s">
+        <v>971</v>
+      </c>
+      <c r="D543" s="41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="544" spans="2:15" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C544" s="42" t="s">
+        <v>972</v>
+      </c>
+      <c r="D544" s="41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="545" spans="3:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C545" s="42" t="s">
+        <v>973</v>
+      </c>
+      <c r="D545" s="41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="546" spans="3:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C546" s="41" t="s">
+        <v>964</v>
+      </c>
+      <c r="D546" s="41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="547" spans="3:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C547" s="41" t="s">
+        <v>966</v>
+      </c>
+      <c r="D547" s="41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="548" spans="3:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C548" s="41" t="s">
+        <v>967</v>
+      </c>
+      <c r="D548" s="41" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="549" spans="3:4" s="41" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="C549" s="41" t="s">
+        <v>968</v>
+      </c>
+      <c r="D549" s="41" t="s">
+        <v>102</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AA484"/>
+  <autoFilter ref="A1:AA549"/>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D243" sqref="D243"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AA594"/>
-    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="130" filter="1" showAutoFilter="1" hiddenRows="1">
       <selection activeCell="E10" sqref="E10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -15981,6 +17217,12 @@
           </filters>
         </filterColumn>
       </autoFilter>
+    </customSheetView>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D243" sqref="D243"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AA594"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="D152">
@@ -16076,12 +17318,12 @@
     <sortCondition ref="B2"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16183,12 +17425,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16273,12 +17515,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -16290,77 +17532,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_dlc_DocId xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">Z7QZ4QWJDNQ7-73874190-17</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">
-      <Url>https://jcp.sharepoint.com/sites/SPOProjects/JCPDotcomPortfolio/AssortmentExpansion/_layouts/15/DocIdRedir.aspx?ID=Z7QZ4QWJDNQ7-73874190-17</Url>
-      <Description>Z7QZ4QWJDNQ7-73874190-17</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10001</Type>
-    <SequenceNumber>1000</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10002</Type>
-    <SequenceNumber>1001</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10004</Type>
-    <SequenceNumber>1002</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-  <Receiver>
-    <Name>Document ID Generator</Name>
-    <Synchronization>Synchronous</Synchronization>
-    <Type>10006</Type>
-    <SequenceNumber>1003</SequenceNumber>
-    <Url/>
-    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
-    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
-    <Data/>
-    <Filter/>
-  </Receiver>
-</spe:Receivers>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003CF273DB610BE64D8338C714685CCF46" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2352d1590348b4df6d1de565ccbd102a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0fff5a07-2326-481b-a4e9-87ff7a79f8dd" xmlns:ns3="2e2046eb-f52d-433a-aad8-97c651e3992c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b5c0a0cba47b5c64de8255dd546e4ec9" ns2:_="" ns3:_="">
     <xsd:import namespace="0fff5a07-2326-481b-a4e9-87ff7a79f8dd"/>
@@ -16538,33 +17709,78 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E9ADEF4-6C25-4BA4-9EDB-E28F722B8411}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="0fff5a07-2326-481b-a4e9-87ff7a79f8dd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_dlc_DocId xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">Z7QZ4QWJDNQ7-73874190-17</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="0fff5a07-2326-481b-a4e9-87ff7a79f8dd">
+      <Url>https://jcp.sharepoint.com/sites/SPOProjects/JCPDotcomPortfolio/AssortmentExpansion/_layouts/15/DocIdRedir.aspx?ID=Z7QZ4QWJDNQ7-73874190-17</Url>
+      <Description>Z7QZ4QWJDNQ7-73874190-17</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{544FA98A-5D89-41A3-B3E3-9D6D7A4BCA0D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A58437D0-211E-4689-9BB7-1D7150BF8997}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<spe:Receivers xmlns:spe="http://schemas.microsoft.com/sharepoint/events">
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10001</Type>
+    <SequenceNumber>1000</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10002</Type>
+    <SequenceNumber>1001</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10004</Type>
+    <SequenceNumber>1002</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+  <Receiver>
+    <Name>Document ID Generator</Name>
+    <Synchronization>Synchronous</Synchronization>
+    <Type>10006</Type>
+    <SequenceNumber>1003</SequenceNumber>
+    <Url/>
+    <Assembly>Microsoft.Office.DocumentManagement, Version=16.0.0.0, Culture=neutral, PublicKeyToken=71e9bce111e9429c</Assembly>
+    <Class>Microsoft.Office.DocumentManagement.Internal.DocIdHandler</Class>
+    <Data/>
+    <Filter/>
+  </Receiver>
+</spe:Receivers>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CAC4C16-FDF5-437E-A8C4-D650CA39502E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -16581,4 +17797,30 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6E9ADEF4-6C25-4BA4-9EDB-E28F722B8411}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="0fff5a07-2326-481b-a4e9-87ff7a79f8dd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{544FA98A-5D89-41A3-B3E3-9D6D7A4BCA0D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A58437D0-211E-4689-9BB7-1D7150BF8997}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/events"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fixed the external names of the relationships. Earlier it was Images for everything
</commit_message>
<xml_diff>
--- a/jcp-dmd/Base Data Model.xlsx
+++ b/jcp-dmd/Base Data Model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19640" tabRatio="500" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19640" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="HELP" sheetId="1" r:id="rId1"/>
@@ -45,8 +45,8 @@
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="Gupta, Kunal - Personal View" guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" tabRatio="500" activeSheetId="4"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" mergeInterval="0" personalView="1" windowWidth="1472" windowHeight="548" tabRatio="500" activeSheetId="4"/>
-    <customWorkbookView name="Gupta, Kunal - Personal View" guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" mergeInterval="0" personalView="1" maximized="1" xWindow="-8" yWindow="-8" windowWidth="1382" windowHeight="744" tabRatio="500" activeSheetId="4"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
@@ -136,7 +136,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3529" uniqueCount="969">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3529" uniqueCount="971">
   <si>
     <t>ACTION</t>
   </si>
@@ -3043,6 +3043,12 @@
   </si>
   <si>
     <t>Ship Point City</t>
+  </si>
+  <si>
+    <t>Videos</t>
+  </si>
+  <si>
+    <t>Documents</t>
   </si>
 </sst>
 </file>
@@ -3907,12 +3913,12 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}">
+      <selection activeCell="B34" sqref="B34"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}">
       <selection activeCell="A5" sqref="A5"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}">
-      <selection activeCell="B34" sqref="B34"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -4083,11 +4089,11 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
       <selection activeCell="B11" sqref="B11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
@@ -4162,14 +4168,14 @@
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="150">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="150">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="150">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -4181,7 +4187,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AF253"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="B93" sqref="B93"/>
@@ -11252,9 +11258,9 @@
   </sheetData>
   <autoFilter ref="A1:AE253"/>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A318" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B322" sqref="B322"/>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1" topLeftCell="E1">
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
       <colBreaks count="1" manualBreakCount="1">
         <brk id="2" max="1048575" man="1"/>
       </colBreaks>
@@ -11262,9 +11268,9 @@
       <pageSetup orientation="portrait" r:id="rId1"/>
       <autoFilter ref="A1:AE347"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1" topLeftCell="E1">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="G109" sqref="G109"/>
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A318" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="B322" sqref="B322"/>
       <colBreaks count="1" manualBreakCount="1">
         <brk id="2" max="1048575" man="1"/>
       </colBreaks>
@@ -11309,9 +11315,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView zoomScale="107" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11578,7 +11584,7 @@
         <v>846</v>
       </c>
       <c r="H11" s="41" t="s">
-        <v>856</v>
+        <v>969</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
@@ -11599,7 +11605,7 @@
         <v>846</v>
       </c>
       <c r="H12" s="41" t="s">
-        <v>856</v>
+        <v>969</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
@@ -11620,7 +11626,7 @@
         <v>846</v>
       </c>
       <c r="H13" s="41" t="s">
-        <v>856</v>
+        <v>969</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
@@ -11641,7 +11647,7 @@
         <v>846</v>
       </c>
       <c r="H14" s="41" t="s">
-        <v>856</v>
+        <v>969</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
@@ -11662,7 +11668,7 @@
         <v>846</v>
       </c>
       <c r="H15" s="41" t="s">
-        <v>856</v>
+        <v>970</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="41" customFormat="1" x14ac:dyDescent="0.2">
@@ -11683,7 +11689,7 @@
         <v>846</v>
       </c>
       <c r="H16" s="41" t="s">
-        <v>856</v>
+        <v>970</v>
       </c>
     </row>
     <row r="17" spans="2:8" s="41" customFormat="1" x14ac:dyDescent="0.2">
@@ -11704,7 +11710,7 @@
         <v>846</v>
       </c>
       <c r="H17" s="41" t="s">
-        <v>856</v>
+        <v>970</v>
       </c>
     </row>
     <row r="18" spans="2:8" s="41" customFormat="1" x14ac:dyDescent="0.2">
@@ -11725,19 +11731,19 @@
         <v>846</v>
       </c>
       <c r="H18" s="41" t="s">
-        <v>856</v>
+        <v>970</v>
       </c>
     </row>
   </sheetData>
   <customSheetViews>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="107">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="107">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="I2" sqref="I2"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-    </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="107">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="C11" sqref="C11"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
   </customSheetViews>
@@ -17149,6 +17155,12 @@
   </sheetData>
   <autoFilter ref="A1:AA541"/>
   <customSheetViews>
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1">
+      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="D243" sqref="D243"/>
+      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+      <autoFilter ref="A1:AA594"/>
+    </customSheetView>
     <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="130" filter="1" showAutoFilter="1" hiddenRows="1">
       <selection activeCell="E10" sqref="E10"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17159,12 +17171,6 @@
           </filters>
         </filterColumn>
       </autoFilter>
-    </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="80" showAutoFilter="1">
-      <pane ySplit="1" topLeftCell="A229" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="D243" sqref="D243"/>
-      <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <autoFilter ref="A1:AA594"/>
     </customSheetView>
   </customSheetViews>
   <conditionalFormatting sqref="D153">
@@ -17260,12 +17266,12 @@
     <sortCondition ref="B2"/>
   </sortState>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="138">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="138">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17367,12 +17373,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E32" sqref="E32"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17457,12 +17463,12 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
+    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
     </customSheetView>
-    <customSheetView guid="{F59B42B5-12A6-408C-8984-297F5E3274B0}" scale="125">
+    <customSheetView guid="{BF8E1B46-AD75-6E4F-85B7-6E6C75F2AAA2}" scale="125">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>